<commit_message>
Changed the mispellings in the spreadsheet (TC -> Tc, rim_categroy -> rim_category).
Continued with the descriptive data coding, where I made the Base Type count better.
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/data_measurements_01.xlsx
+++ b/analysis/data/raw_data/data_measurements_01.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="747">
   <si>
     <t xml:space="preserve">no</t>
   </si>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">size_category</t>
   </si>
   <si>
-    <t xml:space="preserve">rim_categroy</t>
+    <t xml:space="preserve">rim_category</t>
   </si>
   <si>
     <t xml:space="preserve">base_category</t>
@@ -1692,9 +1692,6 @@
   </si>
   <si>
     <t xml:space="preserve">V449</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC</t>
   </si>
   <si>
     <t xml:space="preserve">V450</t>
@@ -26010,7 +26007,7 @@
         <v>22</v>
       </c>
       <c r="H448" t="s">
-        <v>560</v>
+        <v>128</v>
       </c>
       <c r="I448" t="s">
         <v>306</v>
@@ -26049,7 +26046,7 @@
         <v>517</v>
       </c>
       <c r="C449" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D449" t="s">
         <v>519</v>
@@ -26103,7 +26100,7 @@
         <v>517</v>
       </c>
       <c r="C450" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D450" t="s">
         <v>519</v>
@@ -26157,7 +26154,7 @@
         <v>517</v>
       </c>
       <c r="C451" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D451" t="s">
         <v>519</v>
@@ -26209,7 +26206,7 @@
         <v>517</v>
       </c>
       <c r="C452" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D452" t="s">
         <v>519</v>
@@ -26261,7 +26258,7 @@
         <v>517</v>
       </c>
       <c r="C453" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D453" t="s">
         <v>519</v>
@@ -26313,7 +26310,7 @@
         <v>517</v>
       </c>
       <c r="C454" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D454" t="s">
         <v>519</v>
@@ -26365,7 +26362,7 @@
         <v>517</v>
       </c>
       <c r="C455" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D455" t="s">
         <v>519</v>
@@ -26417,7 +26414,7 @@
         <v>517</v>
       </c>
       <c r="C456" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D456" t="s">
         <v>519</v>
@@ -26469,7 +26466,7 @@
         <v>517</v>
       </c>
       <c r="C457" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D457" t="s">
         <v>519</v>
@@ -26521,7 +26518,7 @@
         <v>517</v>
       </c>
       <c r="C458" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D458" t="s">
         <v>519</v>
@@ -26573,7 +26570,7 @@
         <v>517</v>
       </c>
       <c r="C459" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D459" t="s">
         <v>519</v>
@@ -26625,7 +26622,7 @@
         <v>517</v>
       </c>
       <c r="C460" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D460" t="s">
         <v>519</v>
@@ -26677,7 +26674,7 @@
         <v>517</v>
       </c>
       <c r="C461" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D461" t="s">
         <v>519</v>
@@ -26729,7 +26726,7 @@
         <v>517</v>
       </c>
       <c r="C462" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D462" t="s">
         <v>519</v>
@@ -26781,7 +26778,7 @@
         <v>517</v>
       </c>
       <c r="C463" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D463" t="s">
         <v>519</v>
@@ -26833,7 +26830,7 @@
         <v>517</v>
       </c>
       <c r="C464" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D464" t="s">
         <v>519</v>
@@ -26885,7 +26882,7 @@
         <v>517</v>
       </c>
       <c r="C465" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D465" t="s">
         <v>519</v>
@@ -26937,7 +26934,7 @@
         <v>517</v>
       </c>
       <c r="C466" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D466" t="s">
         <v>519</v>
@@ -26989,7 +26986,7 @@
         <v>517</v>
       </c>
       <c r="C467" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D467" t="s">
         <v>519</v>
@@ -27041,7 +27038,7 @@
         <v>517</v>
       </c>
       <c r="C468" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D468" t="s">
         <v>519</v>
@@ -27093,7 +27090,7 @@
         <v>517</v>
       </c>
       <c r="C469" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D469" t="s">
         <v>519</v>
@@ -27147,7 +27144,7 @@
         <v>517</v>
       </c>
       <c r="C470" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D470" t="s">
         <v>519</v>
@@ -27198,13 +27195,13 @@
         <v>472</v>
       </c>
       <c r="B471" t="s">
+        <v>582</v>
+      </c>
+      <c r="C471" t="s">
         <v>583</v>
       </c>
-      <c r="C471" t="s">
+      <c r="D471" t="s">
         <v>584</v>
-      </c>
-      <c r="D471" t="s">
-        <v>585</v>
       </c>
       <c r="E471" t="s">
         <v>43</v>
@@ -27250,13 +27247,13 @@
         <v>473</v>
       </c>
       <c r="B472" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C472" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D472" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E472" t="s">
         <v>43</v>
@@ -27302,13 +27299,13 @@
         <v>474</v>
       </c>
       <c r="B473" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C473" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D473" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E473" t="s">
         <v>43</v>
@@ -27354,13 +27351,13 @@
         <v>475</v>
       </c>
       <c r="B474" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C474" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D474" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E474" t="s">
         <v>43</v>
@@ -27408,13 +27405,13 @@
         <v>476</v>
       </c>
       <c r="B475" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C475" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D475" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E475" t="s">
         <v>43</v>
@@ -27460,13 +27457,13 @@
         <v>477</v>
       </c>
       <c r="B476" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C476" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D476" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E476" t="s">
         <v>43</v>
@@ -27516,13 +27513,13 @@
         <v>478</v>
       </c>
       <c r="B477" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C477" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D477" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E477" t="s">
         <v>43</v>
@@ -27572,13 +27569,13 @@
         <v>479</v>
       </c>
       <c r="B478" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C478" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D478" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E478" t="s">
         <v>43</v>
@@ -27626,13 +27623,13 @@
         <v>480</v>
       </c>
       <c r="B479" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C479" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D479" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E479" t="s">
         <v>43</v>
@@ -27678,13 +27675,13 @@
         <v>481</v>
       </c>
       <c r="B480" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C480" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D480" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E480" t="s">
         <v>43</v>
@@ -27730,13 +27727,13 @@
         <v>482</v>
       </c>
       <c r="B481" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C481" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D481" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E481" t="s">
         <v>43</v>
@@ -27784,13 +27781,13 @@
         <v>483</v>
       </c>
       <c r="B482" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C482" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D482" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E482" t="s">
         <v>43</v>
@@ -27838,13 +27835,13 @@
         <v>484</v>
       </c>
       <c r="B483" t="s">
+        <v>596</v>
+      </c>
+      <c r="C483" t="s">
         <v>597</v>
       </c>
-      <c r="C483" t="s">
+      <c r="D483" t="s">
         <v>598</v>
-      </c>
-      <c r="D483" t="s">
-        <v>599</v>
       </c>
       <c r="E483" t="s">
         <v>21</v>
@@ -27890,13 +27887,13 @@
         <v>485</v>
       </c>
       <c r="B484" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C484" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D484" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E484" t="s">
         <v>21</v>
@@ -27942,13 +27939,13 @@
         <v>486</v>
       </c>
       <c r="B485" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C485" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D485" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E485" t="s">
         <v>21</v>
@@ -27994,13 +27991,13 @@
         <v>487</v>
       </c>
       <c r="B486" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C486" t="s">
+        <v>601</v>
+      </c>
+      <c r="D486" t="s">
         <v>602</v>
-      </c>
-      <c r="D486" t="s">
-        <v>603</v>
       </c>
       <c r="E486" t="s">
         <v>43</v>
@@ -28048,13 +28045,13 @@
         <v>488</v>
       </c>
       <c r="B487" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C487" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D487" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E487" t="s">
         <v>43</v>
@@ -28102,13 +28099,13 @@
         <v>489</v>
       </c>
       <c r="B488" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C488" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D488" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E488" t="s">
         <v>43</v>
@@ -28158,13 +28155,13 @@
         <v>490</v>
       </c>
       <c r="B489" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C489" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D489" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E489" t="s">
         <v>43</v>
@@ -28210,13 +28207,13 @@
         <v>491</v>
       </c>
       <c r="B490" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C490" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D490" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E490" t="s">
         <v>43</v>
@@ -28264,13 +28261,13 @@
         <v>492</v>
       </c>
       <c r="B491" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C491" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D491" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E491" t="s">
         <v>43</v>
@@ -28318,13 +28315,13 @@
         <v>493</v>
       </c>
       <c r="B492" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C492" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D492" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E492" t="s">
         <v>43</v>
@@ -28372,13 +28369,13 @@
         <v>494</v>
       </c>
       <c r="B493" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C493" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D493" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E493" t="s">
         <v>43</v>
@@ -28426,13 +28423,13 @@
         <v>495</v>
       </c>
       <c r="B494" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C494" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D494" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E494" t="s">
         <v>43</v>
@@ -28480,13 +28477,13 @@
         <v>496</v>
       </c>
       <c r="B495" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C495" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D495" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E495" t="s">
         <v>43</v>
@@ -28534,13 +28531,13 @@
         <v>497</v>
       </c>
       <c r="B496" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C496" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D496" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E496" t="s">
         <v>43</v>
@@ -28588,13 +28585,13 @@
         <v>498</v>
       </c>
       <c r="B497" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C497" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D497" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E497" t="s">
         <v>43</v>
@@ -28642,13 +28639,13 @@
         <v>499</v>
       </c>
       <c r="B498" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C498" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D498" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E498" t="s">
         <v>43</v>
@@ -28696,13 +28693,13 @@
         <v>500</v>
       </c>
       <c r="B499" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C499" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D499" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E499" t="s">
         <v>43</v>
@@ -28750,13 +28747,13 @@
         <v>501</v>
       </c>
       <c r="B500" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C500" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D500" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E500" t="s">
         <v>43</v>
@@ -28802,13 +28799,13 @@
         <v>502</v>
       </c>
       <c r="B501" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C501" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D501" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E501" t="s">
         <v>43</v>
@@ -28856,13 +28853,13 @@
         <v>503</v>
       </c>
       <c r="B502" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C502" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D502" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E502" t="s">
         <v>43</v>
@@ -28908,13 +28905,13 @@
         <v>504</v>
       </c>
       <c r="B503" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C503" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D503" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E503" t="s">
         <v>43</v>
@@ -28960,13 +28957,13 @@
         <v>505</v>
       </c>
       <c r="B504" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C504" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D504" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E504" t="s">
         <v>43</v>
@@ -29014,13 +29011,13 @@
         <v>506</v>
       </c>
       <c r="B505" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C505" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D505" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E505" t="s">
         <v>43</v>
@@ -29068,13 +29065,13 @@
         <v>507</v>
       </c>
       <c r="B506" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C506" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D506" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E506" t="s">
         <v>43</v>
@@ -29122,13 +29119,13 @@
         <v>508</v>
       </c>
       <c r="B507" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C507" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D507" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E507" t="s">
         <v>43</v>
@@ -29176,13 +29173,13 @@
         <v>509</v>
       </c>
       <c r="B508" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C508" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D508" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E508" t="s">
         <v>43</v>
@@ -29230,13 +29227,13 @@
         <v>510</v>
       </c>
       <c r="B509" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C509" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D509" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E509" t="s">
         <v>43</v>
@@ -29284,13 +29281,13 @@
         <v>511</v>
       </c>
       <c r="B510" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C510" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D510" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E510" t="s">
         <v>43</v>
@@ -29338,13 +29335,13 @@
         <v>512</v>
       </c>
       <c r="B511" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C511" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D511" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E511" t="s">
         <v>43</v>
@@ -29392,13 +29389,13 @@
         <v>513</v>
       </c>
       <c r="B512" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C512" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D512" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E512" t="s">
         <v>43</v>
@@ -29446,13 +29443,13 @@
         <v>514</v>
       </c>
       <c r="B513" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C513" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D513" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E513" t="s">
         <v>43</v>
@@ -29500,13 +29497,13 @@
         <v>515</v>
       </c>
       <c r="B514" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C514" t="s">
+        <v>630</v>
+      </c>
+      <c r="D514" t="s">
         <v>631</v>
-      </c>
-      <c r="D514" t="s">
-        <v>632</v>
       </c>
       <c r="E514" t="s">
         <v>43</v>
@@ -29554,13 +29551,13 @@
         <v>516</v>
       </c>
       <c r="B515" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C515" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D515" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E515" t="s">
         <v>43</v>
@@ -29608,13 +29605,13 @@
         <v>517</v>
       </c>
       <c r="B516" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C516" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D516" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E516" t="s">
         <v>43</v>
@@ -29662,13 +29659,13 @@
         <v>518</v>
       </c>
       <c r="B517" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C517" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D517" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E517" t="s">
         <v>43</v>
@@ -29716,13 +29713,13 @@
         <v>519</v>
       </c>
       <c r="B518" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C518" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D518" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E518" t="s">
         <v>43</v>
@@ -29770,13 +29767,13 @@
         <v>520</v>
       </c>
       <c r="B519" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C519" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D519" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E519" t="s">
         <v>43</v>
@@ -29824,13 +29821,13 @@
         <v>521</v>
       </c>
       <c r="B520" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C520" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D520" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E520" t="s">
         <v>43</v>
@@ -29878,13 +29875,13 @@
         <v>522</v>
       </c>
       <c r="B521" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C521" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D521" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E521" t="s">
         <v>43</v>
@@ -29932,13 +29929,13 @@
         <v>523</v>
       </c>
       <c r="B522" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C522" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D522" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E522" t="s">
         <v>43</v>
@@ -29986,13 +29983,13 @@
         <v>524</v>
       </c>
       <c r="B523" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C523" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D523" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E523" t="s">
         <v>43</v>
@@ -30040,13 +30037,13 @@
         <v>525</v>
       </c>
       <c r="B524" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C524" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D524" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E524" t="s">
         <v>43</v>
@@ -30094,13 +30091,13 @@
         <v>526</v>
       </c>
       <c r="B525" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C525" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D525" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E525" t="s">
         <v>43</v>
@@ -30148,13 +30145,13 @@
         <v>527</v>
       </c>
       <c r="B526" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C526" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D526" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E526" t="s">
         <v>43</v>
@@ -30202,13 +30199,13 @@
         <v>528</v>
       </c>
       <c r="B527" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C527" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D527" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E527" t="s">
         <v>43</v>
@@ -30223,7 +30220,7 @@
         <v>23</v>
       </c>
       <c r="I527" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J527"/>
       <c r="K527" t="s">
@@ -30256,13 +30253,13 @@
         <v>529</v>
       </c>
       <c r="B528" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C528" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D528" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E528" t="s">
         <v>43</v>
@@ -30277,7 +30274,7 @@
         <v>35</v>
       </c>
       <c r="I528" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J528"/>
       <c r="K528" t="s">
@@ -30310,13 +30307,13 @@
         <v>530</v>
       </c>
       <c r="B529" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C529" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D529" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E529" t="s">
         <v>43</v>
@@ -30364,13 +30361,13 @@
         <v>531</v>
       </c>
       <c r="B530" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C530" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D530" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E530" t="s">
         <v>43</v>
@@ -30418,13 +30415,13 @@
         <v>532</v>
       </c>
       <c r="B531" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C531" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D531" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E531" t="s">
         <v>43</v>
@@ -30470,13 +30467,13 @@
         <v>533</v>
       </c>
       <c r="B532" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C532" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D532" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E532" t="s">
         <v>43</v>
@@ -30524,13 +30521,13 @@
         <v>534</v>
       </c>
       <c r="B533" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C533" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D533" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E533" t="s">
         <v>43</v>
@@ -30578,13 +30575,13 @@
         <v>535</v>
       </c>
       <c r="B534" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C534" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D534" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E534" t="s">
         <v>43</v>
@@ -30599,7 +30596,7 @@
         <v>99</v>
       </c>
       <c r="I534" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J534"/>
       <c r="K534" t="s">
@@ -30632,13 +30629,13 @@
         <v>536</v>
       </c>
       <c r="B535" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C535" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D535" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E535" t="s">
         <v>43</v>
@@ -30684,13 +30681,13 @@
         <v>537</v>
       </c>
       <c r="B536" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C536" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D536" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E536" t="s">
         <v>43</v>
@@ -30736,13 +30733,13 @@
         <v>538</v>
       </c>
       <c r="B537" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C537" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D537" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E537" t="s">
         <v>43</v>
@@ -30788,13 +30785,13 @@
         <v>539</v>
       </c>
       <c r="B538" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C538" t="s">
+        <v>656</v>
+      </c>
+      <c r="D538" t="s">
         <v>657</v>
-      </c>
-      <c r="D538" t="s">
-        <v>658</v>
       </c>
       <c r="E538" t="s">
         <v>43</v>
@@ -30840,13 +30837,13 @@
         <v>540</v>
       </c>
       <c r="B539" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C539" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D539" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E539" t="s">
         <v>43</v>
@@ -30892,13 +30889,13 @@
         <v>541</v>
       </c>
       <c r="B540" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C540" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D540" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E540" t="s">
         <v>43</v>
@@ -30944,13 +30941,13 @@
         <v>542</v>
       </c>
       <c r="B541" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C541" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D541" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E541" t="s">
         <v>43</v>
@@ -30996,13 +30993,13 @@
         <v>543</v>
       </c>
       <c r="B542" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C542" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D542" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E542" t="s">
         <v>43</v>
@@ -31048,13 +31045,13 @@
         <v>544</v>
       </c>
       <c r="B543" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C543" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D543" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E543" t="s">
         <v>43</v>
@@ -31102,13 +31099,13 @@
         <v>545</v>
       </c>
       <c r="B544" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C544" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D544" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E544" t="s">
         <v>43</v>
@@ -31156,13 +31153,13 @@
         <v>546</v>
       </c>
       <c r="B545" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C545" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D545" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E545" t="s">
         <v>43</v>
@@ -31208,13 +31205,13 @@
         <v>547</v>
       </c>
       <c r="B546" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C546" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D546" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E546" t="s">
         <v>43</v>
@@ -31260,13 +31257,13 @@
         <v>548</v>
       </c>
       <c r="B547" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C547" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D547" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E547" t="s">
         <v>43</v>
@@ -31312,13 +31309,13 @@
         <v>549</v>
       </c>
       <c r="B548" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C548" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D548" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E548" t="s">
         <v>43</v>
@@ -31364,13 +31361,13 @@
         <v>550</v>
       </c>
       <c r="B549" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C549" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D549" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E549" t="s">
         <v>43</v>
@@ -31416,13 +31413,13 @@
         <v>551</v>
       </c>
       <c r="B550" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C550" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D550" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E550" t="s">
         <v>43</v>
@@ -31468,13 +31465,13 @@
         <v>552</v>
       </c>
       <c r="B551" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C551" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D551" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E551" t="s">
         <v>43</v>
@@ -31522,13 +31519,13 @@
         <v>553</v>
       </c>
       <c r="B552" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C552" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D552" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E552" t="s">
         <v>43</v>
@@ -31576,13 +31573,13 @@
         <v>554</v>
       </c>
       <c r="B553" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C553" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D553" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E553" t="s">
         <v>43</v>
@@ -31628,10 +31625,10 @@
         <v>555</v>
       </c>
       <c r="B554" t="s">
+        <v>673</v>
+      </c>
+      <c r="C554" t="s">
         <v>674</v>
-      </c>
-      <c r="C554" t="s">
-        <v>675</v>
       </c>
       <c r="D554" t="s">
         <v>404</v>
@@ -31680,10 +31677,10 @@
         <v>556</v>
       </c>
       <c r="B555" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C555" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D555" t="s">
         <v>404</v>
@@ -31732,10 +31729,10 @@
         <v>557</v>
       </c>
       <c r="B556" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C556" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D556" t="s">
         <v>404</v>
@@ -31784,10 +31781,10 @@
         <v>558</v>
       </c>
       <c r="B557" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C557" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D557" t="s">
         <v>404</v>
@@ -31840,10 +31837,10 @@
         <v>560</v>
       </c>
       <c r="B558" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C558" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D558" t="s">
         <v>404</v>
@@ -31894,10 +31891,10 @@
         <v>561</v>
       </c>
       <c r="B559" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C559" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D559" t="s">
         <v>404</v>
@@ -31948,10 +31945,10 @@
         <v>562</v>
       </c>
       <c r="B560" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C560" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D560" t="s">
         <v>404</v>
@@ -32000,10 +31997,10 @@
         <v>563</v>
       </c>
       <c r="B561" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C561" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D561" t="s">
         <v>404</v>
@@ -32052,10 +32049,10 @@
         <v>564</v>
       </c>
       <c r="B562" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C562" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D562" t="s">
         <v>404</v>
@@ -32106,10 +32103,10 @@
         <v>565</v>
       </c>
       <c r="B563" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C563" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D563" t="s">
         <v>404</v>
@@ -32124,7 +32121,7 @@
         <v>22</v>
       </c>
       <c r="H563" t="s">
-        <v>560</v>
+        <v>128</v>
       </c>
       <c r="I563" t="s">
         <v>306</v>
@@ -32160,10 +32157,10 @@
         <v>566</v>
       </c>
       <c r="B564" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C564" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D564" t="s">
         <v>404</v>
@@ -32214,10 +32211,10 @@
         <v>567</v>
       </c>
       <c r="B565" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C565" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D565" t="s">
         <v>404</v>
@@ -32268,10 +32265,10 @@
         <v>568</v>
       </c>
       <c r="B566" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C566" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D566" t="s">
         <v>404</v>
@@ -32322,10 +32319,10 @@
         <v>569</v>
       </c>
       <c r="B567" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C567" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D567" t="s">
         <v>404</v>
@@ -32374,10 +32371,10 @@
         <v>570</v>
       </c>
       <c r="B568" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C568" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D568" t="s">
         <v>404</v>
@@ -32428,13 +32425,13 @@
         <v>571</v>
       </c>
       <c r="B569" t="s">
+        <v>689</v>
+      </c>
+      <c r="C569" t="s">
         <v>690</v>
       </c>
-      <c r="C569" t="s">
+      <c r="D569" t="s">
         <v>691</v>
-      </c>
-      <c r="D569" t="s">
-        <v>692</v>
       </c>
       <c r="E569" t="s">
         <v>21</v>
@@ -32470,13 +32467,13 @@
         <v>572</v>
       </c>
       <c r="B570" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C570" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D570" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E570" t="s">
         <v>21</v>
@@ -32512,13 +32509,13 @@
         <v>573</v>
       </c>
       <c r="B571" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C571" t="s">
+        <v>693</v>
+      </c>
+      <c r="D571" t="s">
         <v>694</v>
-      </c>
-      <c r="D571" t="s">
-        <v>695</v>
       </c>
       <c r="E571" t="s">
         <v>21</v>
@@ -32554,13 +32551,13 @@
         <v>574</v>
       </c>
       <c r="B572" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C572" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D572" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E572" t="s">
         <v>21</v>
@@ -32596,13 +32593,13 @@
         <v>575</v>
       </c>
       <c r="B573" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C573" t="s">
+        <v>696</v>
+      </c>
+      <c r="D573" t="s">
         <v>697</v>
-      </c>
-      <c r="D573" t="s">
-        <v>698</v>
       </c>
       <c r="E573" t="s">
         <v>21</v>
@@ -32638,13 +32635,13 @@
         <v>576</v>
       </c>
       <c r="B574" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C574" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D574" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E574" t="s">
         <v>21</v>
@@ -32680,13 +32677,13 @@
         <v>577</v>
       </c>
       <c r="B575" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C575" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D575" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E575" t="s">
         <v>21</v>
@@ -32722,13 +32719,13 @@
         <v>578</v>
       </c>
       <c r="B576" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C576" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D576" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E576" t="s">
         <v>21</v>
@@ -32764,13 +32761,13 @@
         <v>579</v>
       </c>
       <c r="B577" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C577" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D577" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E577" t="s">
         <v>21</v>
@@ -32806,13 +32803,13 @@
         <v>580</v>
       </c>
       <c r="B578" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C578" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D578" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E578" t="s">
         <v>21</v>
@@ -32848,13 +32845,13 @@
         <v>581</v>
       </c>
       <c r="B579" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C579" t="s">
+        <v>703</v>
+      </c>
+      <c r="D579" t="s">
         <v>704</v>
-      </c>
-      <c r="D579" t="s">
-        <v>705</v>
       </c>
       <c r="E579" t="s">
         <v>21</v>
@@ -32890,13 +32887,13 @@
         <v>582</v>
       </c>
       <c r="B580" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C580" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D580" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E580" t="s">
         <v>21</v>
@@ -32932,13 +32929,13 @@
         <v>583</v>
       </c>
       <c r="B581" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C581" t="s">
+        <v>706</v>
+      </c>
+      <c r="D581" t="s">
         <v>707</v>
-      </c>
-      <c r="D581" t="s">
-        <v>708</v>
       </c>
       <c r="E581" t="s">
         <v>21</v>
@@ -32974,13 +32971,13 @@
         <v>584</v>
       </c>
       <c r="B582" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C582" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D582" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E582" t="s">
         <v>21</v>
@@ -33016,13 +33013,13 @@
         <v>585</v>
       </c>
       <c r="B583" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C583" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D583" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E583" t="s">
         <v>21</v>
@@ -33058,13 +33055,13 @@
         <v>586</v>
       </c>
       <c r="B584" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C584" t="s">
+        <v>710</v>
+      </c>
+      <c r="D584" t="s">
         <v>711</v>
-      </c>
-      <c r="D584" t="s">
-        <v>712</v>
       </c>
       <c r="E584" t="s">
         <v>21</v>
@@ -33100,13 +33097,13 @@
         <v>587</v>
       </c>
       <c r="B585" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C585" t="s">
+        <v>712</v>
+      </c>
+      <c r="D585" t="s">
         <v>713</v>
-      </c>
-      <c r="D585" t="s">
-        <v>714</v>
       </c>
       <c r="E585" t="s">
         <v>21</v>
@@ -33142,13 +33139,13 @@
         <v>588</v>
       </c>
       <c r="B586" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C586" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D586" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E586" t="s">
         <v>21</v>
@@ -33184,13 +33181,13 @@
         <v>589</v>
       </c>
       <c r="B587" t="s">
+        <v>715</v>
+      </c>
+      <c r="C587" t="s">
         <v>716</v>
       </c>
-      <c r="C587" t="s">
+      <c r="D587" t="s">
         <v>717</v>
-      </c>
-      <c r="D587" t="s">
-        <v>718</v>
       </c>
       <c r="E587" t="s">
         <v>21</v>
@@ -33224,13 +33221,13 @@
         <v>590</v>
       </c>
       <c r="B588" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C588" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D588" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E588" t="s">
         <v>21</v>
@@ -33264,13 +33261,13 @@
         <v>591</v>
       </c>
       <c r="B589" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C589" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D589" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E589" t="s">
         <v>21</v>
@@ -33304,13 +33301,13 @@
         <v>592</v>
       </c>
       <c r="B590" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C590" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D590" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E590" t="s">
         <v>21</v>
@@ -33344,13 +33341,13 @@
         <v>593</v>
       </c>
       <c r="B591" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C591" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D591" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E591" t="s">
         <v>21</v>
@@ -33384,13 +33381,13 @@
         <v>594</v>
       </c>
       <c r="B592" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C592" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D592" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E592" t="s">
         <v>21</v>
@@ -33424,13 +33421,13 @@
         <v>595</v>
       </c>
       <c r="B593" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C593" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D593" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E593" t="s">
         <v>21</v>
@@ -33464,13 +33461,13 @@
         <v>596</v>
       </c>
       <c r="B594" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C594" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D594" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E594" t="s">
         <v>21</v>
@@ -33504,13 +33501,13 @@
         <v>597</v>
       </c>
       <c r="B595" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C595" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D595" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E595" t="s">
         <v>21</v>
@@ -33544,13 +33541,13 @@
         <v>598</v>
       </c>
       <c r="B596" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C596" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D596" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E596" t="s">
         <v>21</v>
@@ -33584,13 +33581,13 @@
         <v>599</v>
       </c>
       <c r="B597" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C597" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D597" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E597" t="s">
         <v>21</v>
@@ -33624,13 +33621,13 @@
         <v>600</v>
       </c>
       <c r="B598" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C598" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D598" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E598" t="s">
         <v>21</v>
@@ -33664,13 +33661,13 @@
         <v>601</v>
       </c>
       <c r="B599" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C599" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D599" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E599" t="s">
         <v>21</v>
@@ -33704,13 +33701,13 @@
         <v>602</v>
       </c>
       <c r="B600" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C600" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D600" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E600" t="s">
         <v>21</v>
@@ -33744,13 +33741,13 @@
         <v>603</v>
       </c>
       <c r="B601" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C601" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D601" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E601" t="s">
         <v>21</v>
@@ -33784,13 +33781,13 @@
         <v>604</v>
       </c>
       <c r="B602" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C602" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D602" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E602" t="s">
         <v>21</v>
@@ -33824,13 +33821,13 @@
         <v>605</v>
       </c>
       <c r="B603" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C603" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D603" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E603" t="s">
         <v>21</v>
@@ -33864,13 +33861,13 @@
         <v>606</v>
       </c>
       <c r="B604" t="s">
+        <v>734</v>
+      </c>
+      <c r="C604" t="s">
         <v>735</v>
       </c>
-      <c r="C604" t="s">
+      <c r="D604" t="s">
         <v>736</v>
-      </c>
-      <c r="D604" t="s">
-        <v>737</v>
       </c>
       <c r="E604" t="s">
         <v>21</v>
@@ -33916,13 +33913,13 @@
         <v>607</v>
       </c>
       <c r="B605" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C605" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D605" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E605" t="s">
         <v>21</v>
@@ -33968,13 +33965,13 @@
         <v>608</v>
       </c>
       <c r="B606" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C606" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D606" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E606" t="s">
         <v>21</v>
@@ -34020,13 +34017,13 @@
         <v>609</v>
       </c>
       <c r="B607" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C607" t="s">
+        <v>739</v>
+      </c>
+      <c r="D607" t="s">
         <v>740</v>
-      </c>
-      <c r="D607" t="s">
-        <v>741</v>
       </c>
       <c r="E607" t="s">
         <v>21</v>
@@ -34072,13 +34069,13 @@
         <v>610</v>
       </c>
       <c r="B608" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C608" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D608" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E608" t="s">
         <v>21</v>
@@ -34124,13 +34121,13 @@
         <v>611</v>
       </c>
       <c r="B609" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C609" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D609" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E609" t="s">
         <v>21</v>
@@ -34176,13 +34173,13 @@
         <v>612</v>
       </c>
       <c r="B610" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C610" t="s">
+        <v>743</v>
+      </c>
+      <c r="D610" t="s">
         <v>744</v>
-      </c>
-      <c r="D610" t="s">
-        <v>745</v>
       </c>
       <c r="E610" t="s">
         <v>173</v>
@@ -34228,13 +34225,13 @@
         <v>613</v>
       </c>
       <c r="B611" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C611" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D611" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E611" t="s">
         <v>173</v>
@@ -34280,13 +34277,13 @@
         <v>614</v>
       </c>
       <c r="B612" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C612" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D612" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E612" t="s">
         <v>173</v>

</xml_diff>

<commit_message>
Changed the spreadsheet to new data 05_timelinedata. Inlcuded the backward rims and changed all the legends to include this. Plotted the new barplots in the thesis
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/data_measurements_01.xlsx
+++ b/analysis/data/raw_data/data_measurements_01.xlsx
@@ -644,9 +644,6 @@
     <t xml:space="preserve">V122</t>
   </si>
   <si>
-    <t xml:space="preserve">Emg</t>
-  </si>
-  <si>
     <t xml:space="preserve">V123</t>
   </si>
   <si>
@@ -806,7 +803,7 @@
     <t xml:space="preserve">V167</t>
   </si>
   <si>
-    <t xml:space="preserve">I</t>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">URN 4 - Cover for URN 3</t>
@@ -978,6 +975,9 @@
   </si>
   <si>
     <t xml:space="preserve">440-605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ep</t>
   </si>
   <si>
     <t xml:space="preserve">V206</t>
@@ -3188,7 +3188,9 @@
       <c r="U6" t="n">
         <v>1642.56</v>
       </c>
-      <c r="V6"/>
+      <c r="V6" t="n">
+        <v>239314.42176</v>
+      </c>
       <c r="W6"/>
     </row>
     <row r="7">
@@ -3251,7 +3253,9 @@
       <c r="U7" t="n">
         <v>448</v>
       </c>
-      <c r="V7"/>
+      <c r="V7" t="n">
+        <v>37512.5333333333</v>
+      </c>
       <c r="W7"/>
     </row>
     <row r="8">
@@ -3314,7 +3318,9 @@
       <c r="U8" t="n">
         <v>1142.4</v>
       </c>
-      <c r="V8"/>
+      <c r="V8" t="n">
+        <v>130093.4656</v>
+      </c>
       <c r="W8"/>
     </row>
     <row r="9">
@@ -3377,7 +3383,9 @@
       <c r="U9" t="n">
         <v>1123.2</v>
       </c>
-      <c r="V9"/>
+      <c r="V9" t="n">
+        <v>146716.8768</v>
+      </c>
       <c r="W9"/>
     </row>
     <row r="10">
@@ -3442,7 +3450,9 @@
       <c r="U10" t="n">
         <v>107.52</v>
       </c>
-      <c r="V10"/>
+      <c r="V10" t="n">
+        <v>8642.88768</v>
+      </c>
       <c r="W10" t="s">
         <v>52</v>
       </c>
@@ -3509,7 +3519,9 @@
       <c r="U11" t="n">
         <v>396.8</v>
       </c>
-      <c r="V11"/>
+      <c r="V11" t="n">
+        <v>53160.6186666667</v>
+      </c>
       <c r="W11" t="s">
         <v>52</v>
       </c>
@@ -3576,7 +3588,9 @@
       <c r="U12" t="n">
         <v>158.08</v>
       </c>
-      <c r="V12"/>
+      <c r="V12" t="n">
+        <v>13766.0279466667</v>
+      </c>
       <c r="W12" t="s">
         <v>52</v>
       </c>
@@ -4122,7 +4136,9 @@
       <c r="U20" t="n">
         <v>158.4</v>
       </c>
-      <c r="V20"/>
+      <c r="V20" t="n">
+        <v>7958.016</v>
+      </c>
       <c r="W20" t="s">
         <v>63</v>
       </c>
@@ -4258,7 +4274,9 @@
       <c r="U22" t="n">
         <v>708.48</v>
       </c>
-      <c r="V22"/>
+      <c r="V22" t="n">
+        <v>13625.1549866667</v>
+      </c>
       <c r="W22" t="s">
         <v>63</v>
       </c>
@@ -4325,7 +4343,9 @@
       <c r="U23" t="n">
         <v>20</v>
       </c>
-      <c r="V23"/>
+      <c r="V23" t="n">
+        <v>54.4266666666667</v>
+      </c>
       <c r="W23" t="s">
         <v>63</v>
       </c>
@@ -4392,7 +4412,9 @@
       <c r="U24" t="n">
         <v>77.44</v>
       </c>
-      <c r="V24"/>
+      <c r="V24" t="n">
+        <v>5706.19221333333</v>
+      </c>
       <c r="W24" t="s">
         <v>63</v>
       </c>
@@ -4459,7 +4481,9 @@
       <c r="U25" t="n">
         <v>80.64</v>
       </c>
-      <c r="V25"/>
+      <c r="V25" t="n">
+        <v>5671.89504</v>
+      </c>
       <c r="W25" t="s">
         <v>63</v>
       </c>
@@ -4526,7 +4550,9 @@
       <c r="U26" t="n">
         <v>71.68</v>
       </c>
-      <c r="V26"/>
+      <c r="V26" t="n">
+        <v>3841.28341333333</v>
+      </c>
       <c r="W26" t="s">
         <v>63</v>
       </c>
@@ -4593,7 +4619,9 @@
       <c r="U27" t="n">
         <v>164.64</v>
       </c>
-      <c r="V27"/>
+      <c r="V27" t="n">
+        <v>13510.13888</v>
+      </c>
       <c r="W27" t="s">
         <v>63</v>
       </c>
@@ -6132,7 +6160,7 @@
         <v>1000</v>
       </c>
       <c r="I50" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J50" t="s">
         <v>66</v>
@@ -6369,7 +6397,9 @@
       <c r="U53" t="n">
         <v>2704.96</v>
       </c>
-      <c r="V53"/>
+      <c r="V53" t="n">
+        <v>715725.202773333</v>
+      </c>
       <c r="W53" t="s">
         <v>110</v>
       </c>
@@ -6710,7 +6740,9 @@
       <c r="U58" t="n">
         <v>302.4</v>
       </c>
-      <c r="V58"/>
+      <c r="V58" t="n">
+        <v>35449.344</v>
+      </c>
       <c r="W58"/>
     </row>
     <row r="59">
@@ -6775,7 +6807,9 @@
       <c r="U59" t="n">
         <v>276</v>
       </c>
-      <c r="V59"/>
+      <c r="V59" t="n">
+        <v>34665.6</v>
+      </c>
       <c r="W59"/>
     </row>
     <row r="60">
@@ -6840,7 +6874,9 @@
       <c r="U60" t="n">
         <v>436.8</v>
       </c>
-      <c r="V60"/>
+      <c r="V60" t="n">
+        <v>47547.136</v>
+      </c>
       <c r="W60"/>
     </row>
     <row r="61">
@@ -6905,7 +6941,9 @@
       <c r="U61" t="n">
         <v>576</v>
       </c>
-      <c r="V61"/>
+      <c r="V61" t="n">
+        <v>72345.6</v>
+      </c>
       <c r="W61"/>
     </row>
     <row r="62">
@@ -6970,7 +7008,9 @@
       <c r="U62" t="n">
         <v>264</v>
       </c>
-      <c r="V62"/>
+      <c r="V62" t="n">
+        <v>3098.13333333333</v>
+      </c>
       <c r="W62"/>
     </row>
     <row r="63">
@@ -7035,7 +7075,9 @@
       <c r="U63" t="n">
         <v>397.6</v>
       </c>
-      <c r="V63"/>
+      <c r="V63" t="n">
+        <v>5867.19466666666</v>
+      </c>
       <c r="W63"/>
     </row>
     <row r="64">
@@ -7100,7 +7142,9 @@
       <c r="U64" t="n">
         <v>614.72</v>
       </c>
-      <c r="V64"/>
+      <c r="V64" t="n">
+        <v>116327.973546667</v>
+      </c>
       <c r="W64"/>
     </row>
     <row r="65">
@@ -7232,7 +7276,9 @@
       <c r="U66" t="n">
         <v>204</v>
       </c>
-      <c r="V66"/>
+      <c r="V66" t="n">
+        <v>17423.232</v>
+      </c>
       <c r="W66"/>
     </row>
     <row r="67">
@@ -7297,7 +7343,9 @@
       <c r="U67" t="n">
         <v>241.28</v>
       </c>
-      <c r="V67"/>
+      <c r="V67" t="n">
+        <v>21011.3058133333</v>
+      </c>
       <c r="W67"/>
     </row>
     <row r="68">
@@ -7360,7 +7408,9 @@
       <c r="U68" t="n">
         <v>2037.28</v>
       </c>
-      <c r="V68"/>
+      <c r="V68" t="n">
+        <v>365058.845013333</v>
+      </c>
       <c r="W68"/>
     </row>
     <row r="69">
@@ -7529,7 +7579,7 @@
         <v>32</v>
       </c>
       <c r="K71" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L71"/>
       <c r="M71"/>
@@ -7557,7 +7607,9 @@
       <c r="U71" t="n">
         <v>2096.64</v>
       </c>
-      <c r="V71"/>
+      <c r="V71" t="n">
+        <v>393251.38944</v>
+      </c>
       <c r="W71"/>
     </row>
     <row r="72">
@@ -7620,7 +7672,9 @@
       <c r="U72" t="n">
         <v>634.88</v>
       </c>
-      <c r="V72"/>
+      <c r="V72" t="n">
+        <v>65919.1671466667</v>
+      </c>
       <c r="W72"/>
     </row>
     <row r="73">
@@ -7748,7 +7802,9 @@
       <c r="U74" t="n">
         <v>292.32</v>
       </c>
-      <c r="V74"/>
+      <c r="V74" t="n">
+        <v>3689.99402666667</v>
+      </c>
       <c r="W74"/>
     </row>
     <row r="75">
@@ -7813,7 +7869,9 @@
       <c r="U75" t="n">
         <v>149.6</v>
       </c>
-      <c r="V75"/>
+      <c r="V75" t="n">
+        <v>1268.02410666667</v>
+      </c>
       <c r="W75"/>
     </row>
     <row r="76">
@@ -7880,7 +7938,9 @@
       <c r="U76" t="n">
         <v>691.2</v>
       </c>
-      <c r="V76"/>
+      <c r="V76" t="n">
+        <v>104177.664</v>
+      </c>
       <c r="W76"/>
     </row>
     <row r="77">
@@ -8144,7 +8204,9 @@
       <c r="U80" t="n">
         <v>783.36</v>
       </c>
-      <c r="V80"/>
+      <c r="V80" t="n">
+        <v>16203.60576</v>
+      </c>
       <c r="W80" t="s">
         <v>147</v>
       </c>
@@ -8209,7 +8271,9 @@
       <c r="U81" t="n">
         <v>531.36</v>
       </c>
-      <c r="V81"/>
+      <c r="V81" t="n">
+        <v>9064.66922666667</v>
+      </c>
       <c r="W81" t="s">
         <v>147</v>
       </c>
@@ -8274,7 +8338,9 @@
       <c r="U82" t="n">
         <v>544</v>
       </c>
-      <c r="V82"/>
+      <c r="V82" t="n">
+        <v>9378.13333333333</v>
+      </c>
       <c r="W82" t="s">
         <v>147</v>
       </c>
@@ -8305,7 +8371,7 @@
         <v>900</v>
       </c>
       <c r="I83" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J83" t="s">
         <v>27</v>
@@ -8473,7 +8539,9 @@
       <c r="U85" t="n">
         <v>783.52</v>
       </c>
-      <c r="V85"/>
+      <c r="V85" t="n">
+        <v>77415.9547733333</v>
+      </c>
       <c r="W85" t="s">
         <v>147</v>
       </c>
@@ -8741,7 +8809,9 @@
       <c r="U89" t="n">
         <v>332.64</v>
       </c>
-      <c r="V89"/>
+      <c r="V89" t="n">
+        <v>4486.33152</v>
+      </c>
       <c r="W89" t="s">
         <v>147</v>
       </c>
@@ -8806,7 +8876,9 @@
       <c r="U90" t="n">
         <v>337.92</v>
       </c>
-      <c r="V90"/>
+      <c r="V90" t="n">
+        <v>4595.75424</v>
+      </c>
       <c r="W90" t="s">
         <v>147</v>
       </c>
@@ -8843,7 +8915,7 @@
         <v>32</v>
       </c>
       <c r="K91" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="L91"/>
       <c r="M91"/>
@@ -9005,7 +9077,9 @@
       <c r="U93" t="n">
         <v>380.16</v>
       </c>
-      <c r="V93"/>
+      <c r="V93" t="n">
+        <v>5471.136</v>
+      </c>
       <c r="W93" t="s">
         <v>161</v>
       </c>
@@ -9137,7 +9211,9 @@
       <c r="U95" t="n">
         <v>358.4</v>
       </c>
-      <c r="V95"/>
+      <c r="V95" t="n">
+        <v>5007.38730666667</v>
+      </c>
       <c r="W95" t="s">
         <v>161</v>
       </c>
@@ -9269,7 +9345,9 @@
       <c r="U97" t="n">
         <v>115.52</v>
       </c>
-      <c r="V97"/>
+      <c r="V97" t="n">
+        <v>918.923093333333</v>
+      </c>
       <c r="W97" t="s">
         <v>161</v>
       </c>
@@ -9334,7 +9412,9 @@
       <c r="U98" t="n">
         <v>79.2</v>
       </c>
-      <c r="V98"/>
+      <c r="V98" t="n">
+        <v>519.984</v>
+      </c>
       <c r="W98" t="s">
         <v>161</v>
       </c>
@@ -9466,7 +9546,9 @@
       <c r="U100" t="n">
         <v>176</v>
       </c>
-      <c r="V100"/>
+      <c r="V100" t="n">
+        <v>12968.6186666667</v>
+      </c>
       <c r="W100" t="s">
         <v>161</v>
       </c>
@@ -9531,7 +9613,9 @@
       <c r="U101" t="n">
         <v>167.04</v>
       </c>
-      <c r="V101"/>
+      <c r="V101" t="n">
+        <v>1497.55392</v>
+      </c>
       <c r="W101" t="s">
         <v>161</v>
       </c>
@@ -9596,7 +9680,9 @@
       <c r="U102" t="n">
         <v>116.96</v>
       </c>
-      <c r="V102"/>
+      <c r="V102" t="n">
+        <v>919.559466666666</v>
+      </c>
       <c r="W102" t="s">
         <v>161</v>
       </c>
@@ -9661,7 +9747,9 @@
       <c r="U103" t="n">
         <v>184.32</v>
       </c>
-      <c r="V103"/>
+      <c r="V103" t="n">
+        <v>1852.04736</v>
+      </c>
       <c r="W103" t="s">
         <v>161</v>
       </c>
@@ -9793,7 +9881,9 @@
       <c r="U105" t="n">
         <v>151.36</v>
       </c>
-      <c r="V105"/>
+      <c r="V105" t="n">
+        <v>1377.91573333333</v>
+      </c>
       <c r="W105" t="s">
         <v>161</v>
       </c>
@@ -9992,7 +10082,9 @@
       <c r="U108" t="n">
         <v>395.2</v>
       </c>
-      <c r="V108"/>
+      <c r="V108" t="n">
+        <v>5755.36042666667</v>
+      </c>
       <c r="W108" t="s">
         <v>161</v>
       </c>
@@ -10057,7 +10149,9 @@
       <c r="U109" t="n">
         <v>380.48</v>
       </c>
-      <c r="V109"/>
+      <c r="V109" t="n">
+        <v>5295.56394666667</v>
+      </c>
       <c r="W109" t="s">
         <v>161</v>
       </c>
@@ -10193,7 +10287,9 @@
       <c r="U111" t="n">
         <v>238.08</v>
       </c>
-      <c r="V111"/>
+      <c r="V111" t="n">
+        <v>2662.31808</v>
+      </c>
       <c r="W111" t="s">
         <v>187</v>
       </c>
@@ -10260,7 +10356,9 @@
       <c r="U112" t="n">
         <v>217.12</v>
       </c>
-      <c r="V112"/>
+      <c r="V112" t="n">
+        <v>21452.6139733333</v>
+      </c>
       <c r="W112" t="s">
         <v>189</v>
       </c>
@@ -10327,7 +10425,9 @@
       <c r="U113" t="n">
         <v>209.76</v>
       </c>
-      <c r="V113"/>
+      <c r="V113" t="n">
+        <v>2214.74666666667</v>
+      </c>
       <c r="W113" t="s">
         <v>191</v>
       </c>
@@ -10394,7 +10494,9 @@
       <c r="U114" t="n">
         <v>176.8</v>
       </c>
-      <c r="V114"/>
+      <c r="V114" t="n">
+        <v>1558.41130666667</v>
+      </c>
       <c r="W114" t="s">
         <v>193</v>
       </c>
@@ -10461,7 +10563,9 @@
       <c r="U115" t="n">
         <v>182.24</v>
       </c>
-      <c r="V115"/>
+      <c r="V115" t="n">
+        <v>1616.48874666667</v>
+      </c>
       <c r="W115" t="s">
         <v>195</v>
       </c>
@@ -10528,7 +10632,9 @@
       <c r="U116" t="n">
         <v>208</v>
       </c>
-      <c r="V116"/>
+      <c r="V116" t="n">
+        <v>17416.5333333333</v>
+      </c>
       <c r="W116" t="s">
         <v>197</v>
       </c>
@@ -10595,7 +10701,9 @@
       <c r="U117" t="n">
         <v>248</v>
       </c>
-      <c r="V117"/>
+      <c r="V117" t="n">
+        <v>20765.8666666667</v>
+      </c>
       <c r="W117" t="s">
         <v>199</v>
       </c>
@@ -10662,7 +10770,9 @@
       <c r="U118" t="n">
         <v>661.76</v>
       </c>
-      <c r="V118"/>
+      <c r="V118" t="n">
+        <v>97524.0123733333</v>
+      </c>
       <c r="W118" t="s">
         <v>201</v>
       </c>
@@ -10867,7 +10977,9 @@
       <c r="U121" t="n">
         <v>467.84</v>
       </c>
-      <c r="V121"/>
+      <c r="V121" t="n">
+        <v>7356.47573333333</v>
+      </c>
       <c r="W121" t="s">
         <v>185</v>
       </c>
@@ -10934,7 +11046,9 @@
       <c r="U122" t="n">
         <v>246.24</v>
       </c>
-      <c r="V122"/>
+      <c r="V122" t="n">
+        <v>2478.67413333333</v>
+      </c>
       <c r="W122"/>
     </row>
     <row r="123">
@@ -10969,7 +11083,7 @@
         <v>32</v>
       </c>
       <c r="K123" t="s">
-        <v>210</v>
+        <v>78</v>
       </c>
       <c r="L123" t="s">
         <v>140</v>
@@ -10999,7 +11113,9 @@
       <c r="U123" t="n">
         <v>296.64</v>
       </c>
-      <c r="V123"/>
+      <c r="V123" t="n">
+        <v>2962.55232</v>
+      </c>
       <c r="W123"/>
     </row>
     <row r="124">
@@ -11010,7 +11126,7 @@
         <v>181</v>
       </c>
       <c r="C124" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D124" t="s">
         <v>208</v>
@@ -11064,7 +11180,9 @@
       <c r="U124" t="n">
         <v>238.08</v>
       </c>
-      <c r="V124"/>
+      <c r="V124" t="n">
+        <v>24719.68768</v>
+      </c>
       <c r="W124"/>
     </row>
     <row r="125">
@@ -11075,7 +11193,7 @@
         <v>181</v>
       </c>
       <c r="C125" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D125" t="s">
         <v>208</v>
@@ -11142,7 +11260,7 @@
         <v>181</v>
       </c>
       <c r="C126" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D126" t="s">
         <v>208</v>
@@ -11196,7 +11314,9 @@
       <c r="U126" t="n">
         <v>595.2</v>
       </c>
-      <c r="V126"/>
+      <c r="V126" t="n">
+        <v>92698.8288</v>
+      </c>
       <c r="W126"/>
     </row>
     <row r="127">
@@ -11207,7 +11327,7 @@
         <v>181</v>
       </c>
       <c r="C127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D127" t="s">
         <v>208</v>
@@ -11261,7 +11381,9 @@
       <c r="U127" t="n">
         <v>349.92</v>
       </c>
-      <c r="V127"/>
+      <c r="V127" t="n">
+        <v>47465.94816</v>
+      </c>
       <c r="W127"/>
     </row>
     <row r="128">
@@ -11272,7 +11394,7 @@
         <v>181</v>
       </c>
       <c r="C128" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D128" t="s">
         <v>208</v>
@@ -11326,7 +11448,9 @@
       <c r="U128" t="n">
         <v>427.68</v>
       </c>
-      <c r="V128"/>
+      <c r="V128" t="n">
+        <v>70905.92256</v>
+      </c>
       <c r="W128"/>
     </row>
     <row r="129">
@@ -11337,7 +11461,7 @@
         <v>181</v>
       </c>
       <c r="C129" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D129" t="s">
         <v>208</v>
@@ -11404,7 +11528,7 @@
         <v>181</v>
       </c>
       <c r="C130" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D130" t="s">
         <v>208</v>
@@ -11471,7 +11595,7 @@
         <v>181</v>
       </c>
       <c r="C131" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D131" t="s">
         <v>208</v>
@@ -11538,7 +11662,7 @@
         <v>181</v>
       </c>
       <c r="C132" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D132" t="s">
         <v>208</v>
@@ -11605,7 +11729,7 @@
         <v>181</v>
       </c>
       <c r="C133" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D133" t="s">
         <v>208</v>
@@ -11672,7 +11796,7 @@
         <v>181</v>
       </c>
       <c r="C134" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D134" t="s">
         <v>208</v>
@@ -11726,7 +11850,9 @@
       <c r="U134" t="n">
         <v>146.4</v>
       </c>
-      <c r="V134"/>
+      <c r="V134" t="n">
+        <v>1153.008</v>
+      </c>
       <c r="W134"/>
     </row>
     <row r="135">
@@ -11737,7 +11863,7 @@
         <v>181</v>
       </c>
       <c r="C135" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D135" t="s">
         <v>208</v>
@@ -11804,7 +11930,7 @@
         <v>181</v>
       </c>
       <c r="C136" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D136" t="s">
         <v>208</v>
@@ -11858,7 +11984,9 @@
       <c r="U136" t="n">
         <v>276.48</v>
       </c>
-      <c r="V136"/>
+      <c r="V136" t="n">
+        <v>25002.63936</v>
+      </c>
       <c r="W136"/>
     </row>
     <row r="137">
@@ -11869,7 +11997,7 @@
         <v>181</v>
       </c>
       <c r="C137" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D137" t="s">
         <v>208</v>
@@ -11923,7 +12051,9 @@
       <c r="U137" t="n">
         <v>348.16</v>
       </c>
-      <c r="V137"/>
+      <c r="V137" t="n">
+        <v>39647.5323733333</v>
+      </c>
       <c r="W137"/>
     </row>
     <row r="138">
@@ -11934,7 +12064,7 @@
         <v>181</v>
       </c>
       <c r="C138" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D138" t="s">
         <v>208</v>
@@ -11988,7 +12118,9 @@
       <c r="U138" t="n">
         <v>137.6</v>
       </c>
-      <c r="V138"/>
+      <c r="V138" t="n">
+        <v>1192.36266666667</v>
+      </c>
       <c r="W138"/>
     </row>
     <row r="139">
@@ -11999,7 +12131,7 @@
         <v>181</v>
       </c>
       <c r="C139" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D139" t="s">
         <v>208</v>
@@ -12066,10 +12198,10 @@
         <v>181</v>
       </c>
       <c r="C140" t="s">
+        <v>226</v>
+      </c>
+      <c r="D140" t="s">
         <v>227</v>
-      </c>
-      <c r="D140" t="s">
-        <v>228</v>
       </c>
       <c r="E140" t="s">
         <v>51</v>
@@ -12090,7 +12222,7 @@
         <v>35</v>
       </c>
       <c r="K140" t="s">
-        <v>210</v>
+        <v>109</v>
       </c>
       <c r="L140" t="s">
         <v>140</v>
@@ -12120,7 +12252,9 @@
       <c r="U140" t="n">
         <v>255.36</v>
       </c>
-      <c r="V140"/>
+      <c r="V140" t="n">
+        <v>2587.49397333333</v>
+      </c>
       <c r="W140"/>
     </row>
     <row r="141">
@@ -12131,10 +12265,10 @@
         <v>181</v>
       </c>
       <c r="C141" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D141" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E141" t="s">
         <v>51</v>
@@ -12155,7 +12289,7 @@
         <v>35</v>
       </c>
       <c r="K141" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L141" t="s">
         <v>40</v>
@@ -12185,7 +12319,9 @@
       <c r="U141" t="n">
         <v>268.8</v>
       </c>
-      <c r="V141"/>
+      <c r="V141" t="n">
+        <v>2840.23466666667</v>
+      </c>
       <c r="W141"/>
     </row>
     <row r="142">
@@ -12196,10 +12332,10 @@
         <v>181</v>
       </c>
       <c r="C142" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D142" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E142" t="s">
         <v>51</v>
@@ -12263,10 +12399,10 @@
         <v>181</v>
       </c>
       <c r="C143" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D143" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E143" t="s">
         <v>51</v>
@@ -12330,10 +12466,10 @@
         <v>181</v>
       </c>
       <c r="C144" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D144" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E144" t="s">
         <v>51</v>
@@ -12384,7 +12520,9 @@
       <c r="U144" t="n">
         <v>378.88</v>
       </c>
-      <c r="V144"/>
+      <c r="V144" t="n">
+        <v>46952.8302933333</v>
+      </c>
       <c r="W144"/>
     </row>
     <row r="145">
@@ -12395,10 +12533,10 @@
         <v>181</v>
       </c>
       <c r="C145" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D145" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E145" t="s">
         <v>51</v>
@@ -12419,7 +12557,7 @@
         <v>35</v>
       </c>
       <c r="K145" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L145" t="s">
         <v>40</v>
@@ -12462,10 +12600,10 @@
         <v>181</v>
       </c>
       <c r="C146" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D146" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E146" t="s">
         <v>51</v>
@@ -12516,7 +12654,9 @@
       <c r="U146" t="n">
         <v>616.64</v>
       </c>
-      <c r="V146"/>
+      <c r="V146" t="n">
+        <v>97070.6466133333</v>
+      </c>
       <c r="W146"/>
     </row>
     <row r="147">
@@ -12527,10 +12667,10 @@
         <v>181</v>
       </c>
       <c r="C147" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D147" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E147" t="s">
         <v>51</v>
@@ -12581,7 +12721,9 @@
       <c r="U147" t="n">
         <v>292.64</v>
       </c>
-      <c r="V147"/>
+      <c r="V147" t="n">
+        <v>28914.3927466667</v>
+      </c>
       <c r="W147"/>
     </row>
     <row r="148">
@@ -12592,10 +12734,10 @@
         <v>181</v>
       </c>
       <c r="C148" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D148" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E148" t="s">
         <v>51</v>
@@ -12646,7 +12788,9 @@
       <c r="U148" t="n">
         <v>620.8</v>
       </c>
-      <c r="V148"/>
+      <c r="V148" t="n">
+        <v>100844.407466667</v>
+      </c>
       <c r="W148"/>
     </row>
     <row r="149">
@@ -12657,10 +12801,10 @@
         <v>181</v>
       </c>
       <c r="C149" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D149" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E149" t="s">
         <v>51</v>
@@ -12711,7 +12855,9 @@
       <c r="U149" t="n">
         <v>547.2</v>
       </c>
-      <c r="V149"/>
+      <c r="V149" t="n">
+        <v>69644.6976</v>
+      </c>
       <c r="W149"/>
     </row>
     <row r="150">
@@ -12722,10 +12868,10 @@
         <v>181</v>
       </c>
       <c r="C150" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D150" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E150" t="s">
         <v>51</v>
@@ -12776,7 +12922,9 @@
       <c r="U150" t="n">
         <v>449.28</v>
       </c>
-      <c r="V150"/>
+      <c r="V150" t="n">
+        <v>58686.75072</v>
+      </c>
       <c r="W150"/>
     </row>
     <row r="151">
@@ -12787,10 +12935,10 @@
         <v>181</v>
       </c>
       <c r="C151" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D151" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E151" t="s">
         <v>51</v>
@@ -12841,7 +12989,9 @@
       <c r="U151" t="n">
         <v>256</v>
       </c>
-      <c r="V151"/>
+      <c r="V151" t="n">
+        <v>2972.53333333333</v>
+      </c>
       <c r="W151"/>
     </row>
     <row r="152">
@@ -12852,10 +13002,10 @@
         <v>181</v>
       </c>
       <c r="C152" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D152" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E152" t="s">
         <v>51</v>
@@ -12876,7 +13026,7 @@
         <v>35</v>
       </c>
       <c r="K152" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L152" t="s">
         <v>40</v>
@@ -12908,7 +13058,9 @@
       <c r="U152" t="n">
         <v>421.6</v>
       </c>
-      <c r="V152"/>
+      <c r="V152" t="n">
+        <v>6212.10901333333</v>
+      </c>
       <c r="W152"/>
     </row>
     <row r="153">
@@ -12919,10 +13071,10 @@
         <v>181</v>
       </c>
       <c r="C153" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D153" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E153" t="s">
         <v>51</v>
@@ -12946,7 +13098,7 @@
         <v>28</v>
       </c>
       <c r="L153" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M153" t="s">
         <v>100</v>
@@ -12975,7 +13127,9 @@
       <c r="U153" t="n">
         <v>505.92</v>
       </c>
-      <c r="V153"/>
+      <c r="V153" t="n">
+        <v>78794.00448</v>
+      </c>
       <c r="W153"/>
     </row>
     <row r="154">
@@ -12986,10 +13140,10 @@
         <v>181</v>
       </c>
       <c r="C154" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D154" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E154" t="s">
         <v>51</v>
@@ -13042,7 +13196,9 @@
       <c r="U154" t="n">
         <v>589.76</v>
       </c>
-      <c r="V154"/>
+      <c r="V154" t="n">
+        <v>95802.1870933333</v>
+      </c>
       <c r="W154"/>
     </row>
     <row r="155">
@@ -13053,10 +13209,10 @@
         <v>181</v>
       </c>
       <c r="C155" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D155" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E155" t="s">
         <v>51</v>
@@ -13109,7 +13265,9 @@
       <c r="U155" t="n">
         <v>753.28</v>
       </c>
-      <c r="V155"/>
+      <c r="V155" t="n">
+        <v>134979.741013333</v>
+      </c>
       <c r="W155"/>
     </row>
     <row r="156">
@@ -13120,10 +13278,10 @@
         <v>181</v>
       </c>
       <c r="C156" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D156" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E156" t="s">
         <v>51</v>
@@ -13144,7 +13302,7 @@
         <v>35</v>
       </c>
       <c r="K156" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L156" t="s">
         <v>40</v>
@@ -13174,7 +13332,9 @@
       <c r="U156" t="n">
         <v>316.16</v>
       </c>
-      <c r="V156"/>
+      <c r="V156" t="n">
+        <v>3984.90282666667</v>
+      </c>
       <c r="W156"/>
     </row>
     <row r="157">
@@ -13185,10 +13345,10 @@
         <v>181</v>
       </c>
       <c r="C157" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D157" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E157" t="s">
         <v>51</v>
@@ -13239,7 +13399,9 @@
       <c r="U157" t="n">
         <v>288.96</v>
       </c>
-      <c r="V157"/>
+      <c r="V157" t="n">
+        <v>41616.40448</v>
+      </c>
       <c r="W157"/>
     </row>
     <row r="158">
@@ -13250,10 +13412,10 @@
         <v>181</v>
       </c>
       <c r="C158" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D158" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E158" t="s">
         <v>51</v>
@@ -13306,7 +13468,9 @@
       <c r="U158" t="n">
         <v>393.6</v>
       </c>
-      <c r="V158"/>
+      <c r="V158" t="n">
+        <v>54050.2016</v>
+      </c>
       <c r="W158"/>
     </row>
     <row r="159">
@@ -13317,10 +13481,10 @@
         <v>181</v>
       </c>
       <c r="C159" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D159" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E159" t="s">
         <v>51</v>
@@ -13371,7 +13535,9 @@
       <c r="U159" t="n">
         <v>760.48</v>
       </c>
-      <c r="V159"/>
+      <c r="V159" t="n">
+        <v>123534.399146667</v>
+      </c>
       <c r="W159"/>
     </row>
     <row r="160">
@@ -13382,10 +13548,10 @@
         <v>181</v>
       </c>
       <c r="C160" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D160" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E160" t="s">
         <v>51</v>
@@ -13436,7 +13602,9 @@
       <c r="U160" t="n">
         <v>864.96</v>
       </c>
-      <c r="V160"/>
+      <c r="V160" t="n">
+        <v>147749.00736</v>
+      </c>
       <c r="W160"/>
     </row>
     <row r="161">
@@ -13447,10 +13615,10 @@
         <v>181</v>
       </c>
       <c r="C161" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D161" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E161" t="s">
         <v>51</v>
@@ -13471,7 +13639,7 @@
         <v>32</v>
       </c>
       <c r="K161" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L161"/>
       <c r="M161"/>
@@ -13512,10 +13680,10 @@
         <v>181</v>
       </c>
       <c r="C162" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D162" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E162" t="s">
         <v>51</v>
@@ -13577,10 +13745,10 @@
         <v>181</v>
       </c>
       <c r="C163" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D163" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E163" t="s">
         <v>51</v>
@@ -13642,10 +13810,10 @@
         <v>181</v>
       </c>
       <c r="C164" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D164" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E164" t="s">
         <v>51</v>
@@ -13696,7 +13864,9 @@
       <c r="U164" t="n">
         <v>315.52</v>
       </c>
-      <c r="V164"/>
+      <c r="V164" t="n">
+        <v>4104.13909333333</v>
+      </c>
       <c r="W164"/>
     </row>
     <row r="165">
@@ -13707,7 +13877,7 @@
         <v>181</v>
       </c>
       <c r="C165" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D165" t="s">
         <v>208</v>
@@ -13761,9 +13931,11 @@
       <c r="U165" t="n">
         <v>789.6</v>
       </c>
-      <c r="V165"/>
+      <c r="V165" t="n">
+        <v>138843.264</v>
+      </c>
       <c r="W165" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="166">
@@ -13774,10 +13946,10 @@
         <v>181</v>
       </c>
       <c r="C166" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D166" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E166" t="s">
         <v>51</v>
@@ -13828,9 +14000,11 @@
       <c r="U166" t="n">
         <v>4765.6</v>
       </c>
-      <c r="V166"/>
+      <c r="V166" t="n">
+        <v>1284907.42613333</v>
+      </c>
       <c r="W166" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="167">
@@ -13841,7 +14015,7 @@
         <v>181</v>
       </c>
       <c r="C167" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D167" t="s">
         <v>208</v>
@@ -13865,7 +14039,7 @@
         <v>32</v>
       </c>
       <c r="K167" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L167" t="s">
         <v>140</v>
@@ -13895,9 +14069,11 @@
       <c r="U167" t="n">
         <v>1689.6</v>
       </c>
-      <c r="V167"/>
+      <c r="V167" t="n">
+        <v>248997.4784</v>
+      </c>
       <c r="W167" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="168">
@@ -13908,7 +14084,7 @@
         <v>181</v>
       </c>
       <c r="C168" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D168" t="s">
         <v>208</v>
@@ -13932,7 +14108,7 @@
         <v>32</v>
       </c>
       <c r="K168" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L168" t="s">
         <v>40</v>
@@ -13966,7 +14142,7 @@
         <v>18837.7224533333</v>
       </c>
       <c r="W168" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="169">
@@ -13977,7 +14153,7 @@
         <v>181</v>
       </c>
       <c r="C169" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D169" t="s">
         <v>208</v>
@@ -14001,7 +14177,7 @@
         <v>35</v>
       </c>
       <c r="K169" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L169" t="s">
         <v>40</v>
@@ -14035,7 +14211,7 @@
         <v>11027.73024</v>
       </c>
       <c r="W169" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="170">
@@ -14046,7 +14222,7 @@
         <v>181</v>
       </c>
       <c r="C170" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D170" t="s">
         <v>208</v>
@@ -14070,7 +14246,7 @@
         <v>82</v>
       </c>
       <c r="K170" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L170" t="s">
         <v>140</v>
@@ -14100,9 +14276,11 @@
       <c r="U170" t="n">
         <v>422.4</v>
       </c>
-      <c r="V170"/>
+      <c r="V170" t="n">
+        <v>5122.60437333333</v>
+      </c>
       <c r="W170" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="171">
@@ -14113,7 +14291,7 @@
         <v>181</v>
       </c>
       <c r="C171" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D171" t="s">
         <v>208</v>
@@ -14167,9 +14345,11 @@
       <c r="U171" t="n">
         <v>2076.8</v>
       </c>
-      <c r="V171"/>
+      <c r="V171" t="n">
+        <v>382574.250666667</v>
+      </c>
       <c r="W171" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="172">
@@ -14180,10 +14360,10 @@
         <v>181</v>
       </c>
       <c r="C172" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D172" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E172" t="s">
         <v>51</v>
@@ -14234,9 +14414,11 @@
       <c r="U172" t="n">
         <v>4135.04</v>
       </c>
-      <c r="V172"/>
+      <c r="V172" t="n">
+        <v>983323.538773333</v>
+      </c>
       <c r="W172" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="173">
@@ -14247,10 +14429,10 @@
         <v>181</v>
       </c>
       <c r="C173" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D173" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E173" t="s">
         <v>51</v>
@@ -14307,7 +14489,7 @@
         <v>89950.3323733333</v>
       </c>
       <c r="W173" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="174">
@@ -14318,10 +14500,10 @@
         <v>181</v>
       </c>
       <c r="C174" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D174" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E174" t="s">
         <v>51</v>
@@ -14374,9 +14556,11 @@
       <c r="U174" t="n">
         <v>4334.4</v>
       </c>
-      <c r="V174"/>
+      <c r="V174" t="n">
+        <v>936369.1008</v>
+      </c>
       <c r="W174" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="175">
@@ -14387,10 +14571,10 @@
         <v>181</v>
       </c>
       <c r="C175" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D175" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E175" t="s">
         <v>51</v>
@@ -14441,9 +14625,11 @@
       <c r="U175" t="n">
         <v>994.08</v>
       </c>
-      <c r="V175"/>
+      <c r="V175" t="n">
+        <v>181458.03776</v>
+      </c>
       <c r="W175" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="176">
@@ -14454,10 +14640,10 @@
         <v>181</v>
       </c>
       <c r="C176" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D176" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E176" t="s">
         <v>51</v>
@@ -14508,9 +14694,11 @@
       <c r="U176" t="n">
         <v>5614.08</v>
       </c>
-      <c r="V176"/>
+      <c r="V176" t="n">
+        <v>1617094.57408</v>
+      </c>
       <c r="W176" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="177">
@@ -14521,10 +14709,10 @@
         <v>181</v>
       </c>
       <c r="C177" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D177" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E177" t="s">
         <v>51</v>
@@ -14575,9 +14763,11 @@
       <c r="U177" t="n">
         <v>1012</v>
       </c>
-      <c r="V177"/>
+      <c r="V177" t="n">
+        <v>194897.706666667</v>
+      </c>
       <c r="W177" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="178">
@@ -14585,13 +14775,13 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
+        <v>283</v>
+      </c>
+      <c r="C178" t="s">
         <v>284</v>
       </c>
-      <c r="C178" t="s">
+      <c r="D178" t="s">
         <v>285</v>
-      </c>
-      <c r="D178" t="s">
-        <v>286</v>
       </c>
       <c r="E178" t="s">
         <v>51</v>
@@ -14652,13 +14842,13 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C179" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D179" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E179" t="s">
         <v>51</v>
@@ -14679,7 +14869,7 @@
         <v>66</v>
       </c>
       <c r="K179" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L179" t="s">
         <v>40</v>
@@ -14719,13 +14909,13 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C180" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D180" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E180" t="s">
         <v>51</v>
@@ -14746,7 +14936,7 @@
         <v>66</v>
       </c>
       <c r="K180" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L180" t="s">
         <v>40</v>
@@ -14776,7 +14966,9 @@
       <c r="U180" t="n">
         <v>76</v>
       </c>
-      <c r="V180"/>
+      <c r="V180" t="n">
+        <v>447.370453333333</v>
+      </c>
       <c r="W180"/>
     </row>
     <row r="181">
@@ -14784,13 +14976,13 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C181" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D181" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E181" t="s">
         <v>51</v>
@@ -14811,7 +15003,7 @@
         <v>27</v>
       </c>
       <c r="K181" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L181" t="s">
         <v>40</v>
@@ -14851,13 +15043,13 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C182" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D182" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E182" t="s">
         <v>51</v>
@@ -14878,7 +15070,7 @@
         <v>27</v>
       </c>
       <c r="K182" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L182" t="s">
         <v>40</v>
@@ -14918,13 +15110,13 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C183" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D183" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E183" t="s">
         <v>51</v>
@@ -14985,13 +15177,13 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C184" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D184" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E184" t="s">
         <v>51</v>
@@ -15012,7 +15204,7 @@
         <v>27</v>
       </c>
       <c r="K184" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L184" t="s">
         <v>40</v>
@@ -15042,7 +15234,9 @@
       <c r="U184" t="n">
         <v>215.04</v>
       </c>
-      <c r="V184"/>
+      <c r="V184" t="n">
+        <v>2310.77205333333</v>
+      </c>
       <c r="W184"/>
     </row>
     <row r="185">
@@ -15050,13 +15244,13 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C185" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D185" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E185" t="s">
         <v>51</v>
@@ -15077,7 +15271,7 @@
         <v>35</v>
       </c>
       <c r="K185" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L185" t="s">
         <v>40</v>
@@ -15107,7 +15301,9 @@
       <c r="U185" t="n">
         <v>486.4</v>
       </c>
-      <c r="V185"/>
+      <c r="V185" t="n">
+        <v>7931.22133333333</v>
+      </c>
       <c r="W185"/>
     </row>
     <row r="186">
@@ -15115,13 +15311,13 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C186" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D186" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E186" t="s">
         <v>51</v>
@@ -15142,7 +15338,7 @@
         <v>35</v>
       </c>
       <c r="K186" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L186" t="s">
         <v>40</v>
@@ -15182,13 +15378,13 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C187" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D187" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E187" t="s">
         <v>51</v>
@@ -15209,7 +15405,7 @@
         <v>27</v>
       </c>
       <c r="K187" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L187" t="s">
         <v>40</v>
@@ -15249,13 +15445,13 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C188" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D188" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E188" t="s">
         <v>51</v>
@@ -15306,7 +15502,9 @@
       <c r="U188" t="n">
         <v>574.08</v>
       </c>
-      <c r="V188"/>
+      <c r="V188" t="n">
+        <v>10063.8088533333</v>
+      </c>
       <c r="W188"/>
     </row>
     <row r="189">
@@ -15314,13 +15512,13 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C189" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D189" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E189" t="s">
         <v>51</v>
@@ -15381,13 +15579,13 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C190" t="s">
+        <v>299</v>
+      </c>
+      <c r="D190" t="s">
         <v>300</v>
-      </c>
-      <c r="D190" t="s">
-        <v>301</v>
       </c>
       <c r="E190" t="s">
         <v>51</v>
@@ -15408,7 +15606,7 @@
         <v>27</v>
       </c>
       <c r="K190" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L190" t="s">
         <v>40</v>
@@ -15448,13 +15646,13 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C191" t="s">
+        <v>301</v>
+      </c>
+      <c r="D191" t="s">
         <v>302</v>
-      </c>
-      <c r="D191" t="s">
-        <v>303</v>
       </c>
       <c r="E191" t="s">
         <v>51</v>
@@ -15505,7 +15703,9 @@
       <c r="U191" t="n">
         <v>195.36</v>
       </c>
-      <c r="V191"/>
+      <c r="V191" t="n">
+        <v>10796.37504</v>
+      </c>
       <c r="W191"/>
     </row>
     <row r="192">
@@ -15513,13 +15713,13 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C192" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D192" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E192" t="s">
         <v>51</v>
@@ -15540,7 +15740,7 @@
         <v>66</v>
       </c>
       <c r="K192" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L192" t="s">
         <v>40</v>
@@ -15570,7 +15770,9 @@
       <c r="U192" t="n">
         <v>95.68</v>
       </c>
-      <c r="V192"/>
+      <c r="V192" t="n">
+        <v>3685.33845333333</v>
+      </c>
       <c r="W192"/>
     </row>
     <row r="193">
@@ -15578,13 +15780,13 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C193" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D193" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E193" t="s">
         <v>51</v>
@@ -15635,7 +15837,9 @@
       <c r="U193" t="n">
         <v>75.68</v>
       </c>
-      <c r="V193"/>
+      <c r="V193" t="n">
+        <v>5449.76725333333</v>
+      </c>
       <c r="W193"/>
     </row>
     <row r="194">
@@ -15643,13 +15847,13 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C194" t="s">
+        <v>305</v>
+      </c>
+      <c r="D194" t="s">
         <v>306</v>
-      </c>
-      <c r="D194" t="s">
-        <v>307</v>
       </c>
       <c r="E194" t="s">
         <v>51</v>
@@ -15700,7 +15904,9 @@
       <c r="U194" t="n">
         <v>151.04</v>
       </c>
-      <c r="V194"/>
+      <c r="V194" t="n">
+        <v>14923.5575466667</v>
+      </c>
       <c r="W194"/>
     </row>
     <row r="195">
@@ -15708,13 +15914,13 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C195" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D195" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E195" t="s">
         <v>51</v>
@@ -15775,13 +15981,13 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C196" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D196" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E196" t="s">
         <v>51</v>
@@ -15842,13 +16048,13 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C197" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D197" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E197" t="s">
         <v>51</v>
@@ -15899,7 +16105,9 @@
       <c r="U197" t="n">
         <v>330.88</v>
       </c>
-      <c r="V197"/>
+      <c r="V197" t="n">
+        <v>24381.0030933333</v>
+      </c>
       <c r="W197"/>
     </row>
     <row r="198">
@@ -15907,13 +16115,13 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C198" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D198" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E198" t="s">
         <v>51</v>
@@ -15974,13 +16182,13 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C199" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D199" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E199" t="s">
         <v>51</v>
@@ -16001,7 +16209,7 @@
         <v>27</v>
       </c>
       <c r="K199" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L199" t="s">
         <v>40</v>
@@ -16041,13 +16249,13 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C200" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D200" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E200" t="s">
         <v>51</v>
@@ -16108,13 +16316,13 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C201" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D201" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E201" t="s">
         <v>51</v>
@@ -16175,13 +16383,13 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C202" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D202" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E202" t="s">
         <v>51</v>
@@ -16232,7 +16440,9 @@
       <c r="U202" t="n">
         <v>318.24</v>
       </c>
-      <c r="V202"/>
+      <c r="V202" t="n">
+        <v>20784.89088</v>
+      </c>
       <c r="W202"/>
     </row>
     <row r="203">
@@ -16240,13 +16450,13 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C203" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D203" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E203" t="s">
         <v>51</v>
@@ -16307,13 +16517,13 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C204" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D204" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E204" t="s">
         <v>51</v>
@@ -16334,7 +16544,7 @@
         <v>35</v>
       </c>
       <c r="K204" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L204" t="s">
         <v>40</v>
@@ -16364,7 +16574,9 @@
       <c r="U204" t="n">
         <v>727.04</v>
       </c>
-      <c r="V204"/>
+      <c r="V204" t="n">
+        <v>77923.1778133333</v>
+      </c>
       <c r="W204"/>
     </row>
     <row r="205">
@@ -16372,13 +16584,13 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C205" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D205" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E205" t="s">
         <v>51</v>
@@ -16439,13 +16651,13 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C206" t="s">
+        <v>319</v>
+      </c>
+      <c r="D206" t="s">
         <v>320</v>
-      </c>
-      <c r="D206" t="s">
-        <v>321</v>
       </c>
       <c r="E206" t="s">
         <v>51</v>
@@ -16466,7 +16678,7 @@
         <v>35</v>
       </c>
       <c r="K206" t="s">
-        <v>109</v>
+        <v>321</v>
       </c>
       <c r="L206" t="s">
         <v>40</v>
@@ -16506,13 +16718,13 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C207" t="s">
         <v>322</v>
       </c>
       <c r="D207" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E207" t="s">
         <v>51</v>
@@ -16533,7 +16745,7 @@
         <v>32</v>
       </c>
       <c r="K207" t="s">
-        <v>109</v>
+        <v>321</v>
       </c>
       <c r="L207" t="s">
         <v>40</v>
@@ -16573,13 +16785,13 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C208" t="s">
         <v>323</v>
       </c>
       <c r="D208" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E208" t="s">
         <v>51</v>
@@ -16600,7 +16812,7 @@
         <v>35</v>
       </c>
       <c r="K208" t="s">
-        <v>109</v>
+        <v>321</v>
       </c>
       <c r="L208" t="s">
         <v>40</v>
@@ -16630,7 +16842,9 @@
       <c r="U208" t="n">
         <v>783.84</v>
       </c>
-      <c r="V208"/>
+      <c r="V208" t="n">
+        <v>90574.27968</v>
+      </c>
       <c r="W208"/>
     </row>
     <row r="209">
@@ -16638,13 +16852,13 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C209" t="s">
         <v>324</v>
       </c>
       <c r="D209" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E209" t="s">
         <v>51</v>
@@ -16705,13 +16919,13 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C210" t="s">
         <v>326</v>
       </c>
       <c r="D210" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E210" t="s">
         <v>51</v>
@@ -16732,7 +16946,7 @@
         <v>32</v>
       </c>
       <c r="K210" t="s">
-        <v>109</v>
+        <v>321</v>
       </c>
       <c r="L210" t="s">
         <v>40</v>
@@ -16772,13 +16986,13 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C211" t="s">
         <v>327</v>
       </c>
       <c r="D211" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E211" t="s">
         <v>51</v>
@@ -16799,7 +17013,7 @@
         <v>32</v>
       </c>
       <c r="K211" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L211" t="s">
         <v>40</v>
@@ -16839,13 +17053,13 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C212" t="s">
         <v>328</v>
       </c>
       <c r="D212" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E212" t="s">
         <v>51</v>
@@ -16866,7 +17080,7 @@
         <v>32</v>
       </c>
       <c r="K212" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L212" t="s">
         <v>40</v>
@@ -16896,7 +17110,9 @@
       <c r="U212" t="n">
         <v>2433.12</v>
       </c>
-      <c r="V212"/>
+      <c r="V212" t="n">
+        <v>452287.81056</v>
+      </c>
       <c r="W212"/>
     </row>
     <row r="213">
@@ -16904,13 +17120,13 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C213" t="s">
         <v>329</v>
       </c>
       <c r="D213" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E213" t="s">
         <v>51</v>
@@ -16971,13 +17187,13 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C214" t="s">
         <v>330</v>
       </c>
       <c r="D214" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E214" t="s">
         <v>51</v>
@@ -17038,13 +17254,13 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C215" t="s">
         <v>331</v>
       </c>
       <c r="D215" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E215" t="s">
         <v>51</v>
@@ -17105,13 +17321,13 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C216" t="s">
         <v>332</v>
       </c>
       <c r="D216" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E216" t="s">
         <v>51</v>
@@ -17172,13 +17388,13 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C217" t="s">
         <v>333</v>
       </c>
       <c r="D217" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E217" t="s">
         <v>51</v>
@@ -17239,13 +17455,13 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C218" t="s">
         <v>334</v>
       </c>
       <c r="D218" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E218" t="s">
         <v>51</v>
@@ -17306,13 +17522,13 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C219" t="s">
         <v>335</v>
       </c>
       <c r="D219" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E219" t="s">
         <v>51</v>
@@ -17363,7 +17579,9 @@
       <c r="U219" t="n">
         <v>1464.32</v>
       </c>
-      <c r="V219"/>
+      <c r="V219" t="n">
+        <v>215797.814613333</v>
+      </c>
       <c r="W219"/>
     </row>
     <row r="220">
@@ -17371,13 +17589,13 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C220" t="s">
         <v>336</v>
       </c>
       <c r="D220" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E220" t="s">
         <v>51</v>
@@ -17428,7 +17646,9 @@
       <c r="U220" t="n">
         <v>410.4</v>
       </c>
-      <c r="V220"/>
+      <c r="V220" t="n">
+        <v>30927.744</v>
+      </c>
       <c r="W220"/>
     </row>
     <row r="221">
@@ -17436,7 +17656,7 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C221" t="s">
         <v>337</v>
@@ -17503,13 +17723,13 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C222" t="s">
         <v>339</v>
       </c>
       <c r="D222" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E222" t="s">
         <v>51</v>
@@ -17570,13 +17790,13 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C223" t="s">
         <v>340</v>
       </c>
       <c r="D223" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E223" t="s">
         <v>51</v>
@@ -17637,13 +17857,13 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C224" t="s">
         <v>342</v>
       </c>
       <c r="D224" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E224" t="s">
         <v>51</v>
@@ -19356,7 +19576,7 @@
         <v>82</v>
       </c>
       <c r="K250" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L250"/>
       <c r="M250"/>
@@ -20034,7 +20254,9 @@
       <c r="U260" t="n">
         <v>191.52</v>
       </c>
-      <c r="V260"/>
+      <c r="V260" t="n">
+        <v>1905.40224</v>
+      </c>
       <c r="W260"/>
     </row>
     <row r="261">
@@ -20097,7 +20319,9 @@
       <c r="U261" t="n">
         <v>230.4</v>
       </c>
-      <c r="V261"/>
+      <c r="V261" t="n">
+        <v>2546.56512</v>
+      </c>
       <c r="W261"/>
     </row>
     <row r="262">
@@ -20225,7 +20449,9 @@
       <c r="U263" t="n">
         <v>136.8</v>
       </c>
-      <c r="V263"/>
+      <c r="V263" t="n">
+        <v>1172.83605333333</v>
+      </c>
       <c r="W263"/>
     </row>
     <row r="264">
@@ -20288,7 +20514,9 @@
       <c r="U264" t="n">
         <v>228.8</v>
       </c>
-      <c r="V264"/>
+      <c r="V264" t="n">
+        <v>2447.82677333333</v>
+      </c>
       <c r="W264"/>
     </row>
     <row r="265">
@@ -20351,7 +20579,9 @@
       <c r="U265" t="n">
         <v>286.72</v>
       </c>
-      <c r="V265"/>
+      <c r="V265" t="n">
+        <v>3571.19317333333</v>
+      </c>
       <c r="W265"/>
     </row>
     <row r="266">
@@ -20414,7 +20644,9 @@
       <c r="U266" t="n">
         <v>445.44</v>
       </c>
-      <c r="V266"/>
+      <c r="V266" t="n">
+        <v>6756.54314666667</v>
+      </c>
       <c r="W266"/>
     </row>
     <row r="267">
@@ -20477,7 +20709,9 @@
       <c r="U267" t="n">
         <v>160</v>
       </c>
-      <c r="V267"/>
+      <c r="V267" t="n">
+        <v>1473.70666666667</v>
+      </c>
       <c r="W267"/>
     </row>
     <row r="268">
@@ -20540,7 +20774,9 @@
       <c r="U268" t="n">
         <v>252</v>
       </c>
-      <c r="V268"/>
+      <c r="V268" t="n">
+        <v>2909.73333333333</v>
+      </c>
       <c r="W268"/>
     </row>
     <row r="269">
@@ -20603,7 +20839,9 @@
       <c r="U269" t="n">
         <v>360</v>
       </c>
-      <c r="V269"/>
+      <c r="V269" t="n">
+        <v>4973.76</v>
+      </c>
       <c r="W269"/>
     </row>
     <row r="270">
@@ -21483,7 +21721,7 @@
         <v>32</v>
       </c>
       <c r="K283" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L283"/>
       <c r="M283"/>
@@ -21678,7 +21916,7 @@
         <v>35</v>
       </c>
       <c r="K286" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L286"/>
       <c r="M286"/>
@@ -21706,7 +21944,9 @@
       <c r="U286" t="n">
         <v>227.52</v>
       </c>
-      <c r="V286"/>
+      <c r="V286" t="n">
+        <v>2181.21984</v>
+      </c>
       <c r="W286"/>
     </row>
     <row r="287">
@@ -21769,7 +22009,9 @@
       <c r="U287" t="n">
         <v>129.92</v>
       </c>
-      <c r="V287"/>
+      <c r="V287" t="n">
+        <v>958.445226666666</v>
+      </c>
       <c r="W287"/>
     </row>
     <row r="288">
@@ -21832,7 +22074,9 @@
       <c r="U288" t="n">
         <v>153.6</v>
       </c>
-      <c r="V288"/>
+      <c r="V288" t="n">
+        <v>1268.99541333333</v>
+      </c>
       <c r="W288"/>
     </row>
     <row r="289">
@@ -21895,7 +22139,9 @@
       <c r="U289" t="n">
         <v>353.28</v>
       </c>
-      <c r="V289"/>
+      <c r="V289" t="n">
+        <v>4398.61248</v>
+      </c>
       <c r="W289"/>
     </row>
     <row r="290">
@@ -21958,7 +22204,9 @@
       <c r="U290" t="n">
         <v>122.4</v>
       </c>
-      <c r="V290"/>
+      <c r="V290" t="n">
+        <v>926.928</v>
+      </c>
       <c r="W290"/>
     </row>
     <row r="291">
@@ -22021,7 +22269,9 @@
       <c r="U291" t="n">
         <v>61.6</v>
       </c>
-      <c r="V291"/>
+      <c r="V291" t="n">
+        <v>336.373546666667</v>
+      </c>
       <c r="W291"/>
     </row>
     <row r="292">
@@ -22084,7 +22334,9 @@
       <c r="U292" t="n">
         <v>100.8</v>
       </c>
-      <c r="V292"/>
+      <c r="V292" t="n">
+        <v>702.422186666666</v>
+      </c>
       <c r="W292"/>
     </row>
     <row r="293">
@@ -22147,7 +22399,9 @@
       <c r="U293" t="n">
         <v>188.48</v>
       </c>
-      <c r="V293"/>
+      <c r="V293" t="n">
+        <v>1789.48181333333</v>
+      </c>
       <c r="W293"/>
     </row>
     <row r="294">
@@ -22210,7 +22464,9 @@
       <c r="U294" t="n">
         <v>93.6</v>
       </c>
-      <c r="V294"/>
+      <c r="V294" t="n">
+        <v>616.980693333333</v>
+      </c>
       <c r="W294"/>
     </row>
     <row r="295">
@@ -22273,7 +22529,9 @@
       <c r="U295" t="n">
         <v>163.2</v>
       </c>
-      <c r="V295"/>
+      <c r="V295" t="n">
+        <v>1114.12224</v>
+      </c>
       <c r="W295"/>
     </row>
     <row r="296">
@@ -22336,7 +22594,9 @@
       <c r="U296" t="n">
         <v>99.84</v>
       </c>
-      <c r="V296"/>
+      <c r="V296" t="n">
+        <v>636.64128</v>
+      </c>
       <c r="W296"/>
     </row>
     <row r="297">
@@ -22399,7 +22659,9 @@
       <c r="U297" t="n">
         <v>364.8</v>
       </c>
-      <c r="V297"/>
+      <c r="V297" t="n">
+        <v>4572.24192</v>
+      </c>
       <c r="W297"/>
     </row>
     <row r="298">
@@ -22462,7 +22724,9 @@
       <c r="U298" t="n">
         <v>419.52</v>
       </c>
-      <c r="V298"/>
+      <c r="V298" t="n">
+        <v>5244.52010666667</v>
+      </c>
       <c r="W298"/>
     </row>
     <row r="299">
@@ -22525,7 +22789,9 @@
       <c r="U299" t="n">
         <v>281.6</v>
       </c>
-      <c r="V299"/>
+      <c r="V299" t="n">
+        <v>3177.31157333333</v>
+      </c>
       <c r="W299"/>
     </row>
     <row r="300">
@@ -22588,7 +22854,9 @@
       <c r="U300" t="n">
         <v>116.48</v>
       </c>
-      <c r="V300"/>
+      <c r="V300" t="n">
+        <v>840.280746666667</v>
+      </c>
       <c r="W300"/>
     </row>
     <row r="301">
@@ -22651,7 +22919,9 @@
       <c r="U301" t="n">
         <v>228</v>
       </c>
-      <c r="V301"/>
+      <c r="V301" t="n">
+        <v>2261.03445333333</v>
+      </c>
       <c r="W301"/>
     </row>
     <row r="302">
@@ -22714,7 +22984,9 @@
       <c r="U302" t="n">
         <v>201.28</v>
       </c>
-      <c r="V302"/>
+      <c r="V302" t="n">
+        <v>1819.75978666667</v>
+      </c>
       <c r="W302"/>
     </row>
     <row r="303">
@@ -22777,7 +23049,9 @@
       <c r="U303" t="n">
         <v>114.4</v>
       </c>
-      <c r="V303"/>
+      <c r="V303" t="n">
+        <v>786.791893333333</v>
+      </c>
       <c r="W303"/>
     </row>
     <row r="304">
@@ -22840,7 +23114,9 @@
       <c r="U304" t="n">
         <v>148.8</v>
       </c>
-      <c r="V304"/>
+      <c r="V304" t="n">
+        <v>1175.616</v>
+      </c>
       <c r="W304"/>
     </row>
     <row r="305">
@@ -22903,7 +23179,9 @@
       <c r="U305" t="n">
         <v>62.4</v>
       </c>
-      <c r="V305"/>
+      <c r="V305" t="n">
+        <v>362.263893333333</v>
+      </c>
       <c r="W305"/>
     </row>
     <row r="306">
@@ -22966,7 +23244,9 @@
       <c r="U306" t="n">
         <v>67.2</v>
       </c>
-      <c r="V306"/>
+      <c r="V306" t="n">
+        <v>390.66624</v>
+      </c>
       <c r="W306"/>
     </row>
     <row r="307">
@@ -23159,7 +23439,9 @@
       <c r="U309" t="n">
         <v>4646.4</v>
       </c>
-      <c r="V309"/>
+      <c r="V309" t="n">
+        <v>1283893.248</v>
+      </c>
       <c r="W309"/>
     </row>
     <row r="310">
@@ -23222,7 +23504,9 @@
       <c r="U310" t="n">
         <v>876</v>
       </c>
-      <c r="V310"/>
+      <c r="V310" t="n">
+        <v>107091.584</v>
+      </c>
       <c r="W310"/>
     </row>
     <row r="311">
@@ -23395,7 +23679,7 @@
         <v>35</v>
       </c>
       <c r="K313" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L313" t="s">
         <v>40</v>
@@ -23561,7 +23845,9 @@
       <c r="U315" t="n">
         <v>299.52</v>
       </c>
-      <c r="V315"/>
+      <c r="V315" t="n">
+        <v>18057.46176</v>
+      </c>
       <c r="W315" t="s">
         <v>445</v>
       </c>
@@ -23628,7 +23914,9 @@
       <c r="U316" t="n">
         <v>1098.24</v>
       </c>
-      <c r="V316"/>
+      <c r="V316" t="n">
+        <v>121386.27072</v>
+      </c>
       <c r="W316" t="s">
         <v>448</v>
       </c>
@@ -23833,7 +24121,9 @@
       <c r="U319" t="n">
         <v>72</v>
       </c>
-      <c r="V319"/>
+      <c r="V319" t="n">
+        <v>452.16</v>
+      </c>
       <c r="W319" t="s">
         <v>437</v>
       </c>
@@ -24107,7 +24397,9 @@
       <c r="U323" t="n">
         <v>63.36</v>
       </c>
-      <c r="V323"/>
+      <c r="V323" t="n">
+        <v>1909.92384</v>
+      </c>
       <c r="W323" t="s">
         <v>457</v>
       </c>
@@ -24174,7 +24466,9 @@
       <c r="U324" t="n">
         <v>40.8</v>
       </c>
-      <c r="V324"/>
+      <c r="V324" t="n">
+        <v>1024.896</v>
+      </c>
       <c r="W324" t="s">
         <v>457</v>
       </c>
@@ -24241,7 +24535,9 @@
       <c r="U325" t="n">
         <v>36.48</v>
       </c>
-      <c r="V325"/>
+      <c r="V325" t="n">
+        <v>733.10208</v>
+      </c>
       <c r="W325" t="s">
         <v>457</v>
       </c>
@@ -24308,7 +24604,9 @@
       <c r="U326" t="n">
         <v>729.6</v>
       </c>
-      <c r="V326"/>
+      <c r="V326" t="n">
+        <v>73310.208</v>
+      </c>
       <c r="W326" t="s">
         <v>457</v>
       </c>
@@ -24375,7 +24673,9 @@
       <c r="U327" t="n">
         <v>53.76</v>
       </c>
-      <c r="V327"/>
+      <c r="V327" t="n">
+        <v>1440.48128</v>
+      </c>
       <c r="W327" t="s">
         <v>463</v>
       </c>
@@ -24442,7 +24742,9 @@
       <c r="U328" t="n">
         <v>648</v>
       </c>
-      <c r="V328"/>
+      <c r="V328" t="n">
+        <v>54259.2</v>
+      </c>
       <c r="W328" t="s">
         <v>448</v>
       </c>
@@ -24509,7 +24811,9 @@
       <c r="U329" t="n">
         <v>380.16</v>
       </c>
-      <c r="V329"/>
+      <c r="V329" t="n">
+        <v>4803.74784</v>
+      </c>
       <c r="W329" t="s">
         <v>457</v>
       </c>
@@ -24576,7 +24880,9 @@
       <c r="U330" t="n">
         <v>358.56</v>
       </c>
-      <c r="V330"/>
+      <c r="V330" t="n">
+        <v>4761.2448</v>
+      </c>
       <c r="W330" t="s">
         <v>457</v>
       </c>
@@ -24643,7 +24949,9 @@
       <c r="U331" t="n">
         <v>590.4</v>
       </c>
-      <c r="V331"/>
+      <c r="V331" t="n">
+        <v>10584.8311466667</v>
+      </c>
       <c r="W331" t="s">
         <v>457</v>
       </c>
@@ -24710,7 +25018,9 @@
       <c r="U332" t="n">
         <v>92.8</v>
       </c>
-      <c r="V332"/>
+      <c r="V332" t="n">
+        <v>4506.86293333333</v>
+      </c>
       <c r="W332" t="s">
         <v>457</v>
       </c>
@@ -24986,7 +25296,9 @@
       <c r="U336" t="n">
         <v>63.84</v>
       </c>
-      <c r="V336"/>
+      <c r="V336" t="n">
+        <v>2031.30368</v>
+      </c>
       <c r="W336" t="s">
         <v>477</v>
       </c>
@@ -25398,7 +25710,9 @@
       <c r="U342" t="n">
         <v>183.52</v>
       </c>
-      <c r="V342"/>
+      <c r="V342" t="n">
+        <v>9527.37962666667</v>
+      </c>
       <c r="W342" t="s">
         <v>483</v>
       </c>
@@ -25500,7 +25814,7 @@
         <v>1140</v>
       </c>
       <c r="I344" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J344" t="s">
         <v>35</v>
@@ -25713,7 +26027,7 @@
         <v>27</v>
       </c>
       <c r="K347" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L347" t="s">
         <v>40</v>
@@ -25812,7 +26126,9 @@
       <c r="U348" t="n">
         <v>191.36</v>
       </c>
-      <c r="V348"/>
+      <c r="V348" t="n">
+        <v>14741.3538133333</v>
+      </c>
       <c r="W348" t="s">
         <v>483</v>
       </c>
@@ -26080,7 +26396,9 @@
       <c r="U352" t="n">
         <v>134.4</v>
       </c>
-      <c r="V352"/>
+      <c r="V352" t="n">
+        <v>7877.632</v>
+      </c>
       <c r="W352"/>
     </row>
     <row r="353">
@@ -26145,7 +26463,9 @@
       <c r="U353" t="n">
         <v>138.24</v>
       </c>
-      <c r="V353"/>
+      <c r="V353" t="n">
+        <v>7408.18944</v>
+      </c>
       <c r="W353"/>
     </row>
     <row r="354">
@@ -26210,7 +26530,9 @@
       <c r="U354" t="n">
         <v>103.36</v>
       </c>
-      <c r="V354"/>
+      <c r="V354" t="n">
+        <v>5885.18058666667</v>
+      </c>
       <c r="W354"/>
     </row>
     <row r="355">
@@ -26543,7 +26865,9 @@
       <c r="U359" t="n">
         <v>61.6</v>
       </c>
-      <c r="V359"/>
+      <c r="V359" t="n">
+        <v>336.373546666667</v>
+      </c>
       <c r="W359"/>
     </row>
     <row r="360">
@@ -26608,7 +26932,9 @@
       <c r="U360" t="n">
         <v>353.28</v>
       </c>
-      <c r="V360"/>
+      <c r="V360" t="n">
+        <v>40822.21056</v>
+      </c>
       <c r="W360"/>
     </row>
     <row r="361">
@@ -26673,7 +26999,9 @@
       <c r="U361" t="n">
         <v>224.64</v>
       </c>
-      <c r="V361"/>
+      <c r="V361" t="n">
+        <v>13543.09632</v>
+      </c>
       <c r="W361"/>
     </row>
     <row r="362">
@@ -26872,7 +27200,9 @@
       <c r="U364" t="n">
         <v>196.8</v>
       </c>
-      <c r="V364"/>
+      <c r="V364" t="n">
+        <v>13512.5504</v>
+      </c>
       <c r="W364"/>
     </row>
     <row r="365">
@@ -27108,7 +27438,7 @@
         <v>35</v>
       </c>
       <c r="K368" t="s">
-        <v>109</v>
+        <v>321</v>
       </c>
       <c r="L368" t="s">
         <v>40</v>
@@ -27272,7 +27602,9 @@
       <c r="U370" t="n">
         <v>228.48</v>
       </c>
-      <c r="V370"/>
+      <c r="V370" t="n">
+        <v>19514.01984</v>
+      </c>
       <c r="W370"/>
     </row>
     <row r="371">
@@ -27337,7 +27669,9 @@
       <c r="U371" t="n">
         <v>195.52</v>
       </c>
-      <c r="V371"/>
+      <c r="V371" t="n">
+        <v>15389.2488533333</v>
+      </c>
       <c r="W371"/>
     </row>
     <row r="372">
@@ -27402,7 +27736,9 @@
       <c r="U372" t="n">
         <v>194.4</v>
       </c>
-      <c r="V372"/>
+      <c r="V372" t="n">
+        <v>14649.984</v>
+      </c>
       <c r="W372"/>
     </row>
     <row r="373">
@@ -27467,7 +27803,9 @@
       <c r="U373" t="n">
         <v>180</v>
       </c>
-      <c r="V373"/>
+      <c r="V373" t="n">
+        <v>13564.8</v>
+      </c>
       <c r="W373"/>
     </row>
     <row r="374">
@@ -27502,7 +27840,7 @@
         <v>27</v>
       </c>
       <c r="K374" t="s">
-        <v>109</v>
+        <v>321</v>
       </c>
       <c r="L374" t="s">
         <v>40</v>
@@ -27800,7 +28138,9 @@
       <c r="U378" t="n">
         <v>624.16</v>
       </c>
-      <c r="V378"/>
+      <c r="V378" t="n">
+        <v>86756.5755733333</v>
+      </c>
       <c r="W378" t="s">
         <v>529</v>
       </c>
@@ -27936,7 +28276,9 @@
       <c r="U380" t="n">
         <v>144</v>
       </c>
-      <c r="V380"/>
+      <c r="V380" t="n">
+        <v>1214.13333333333</v>
+      </c>
       <c r="W380" t="s">
         <v>529</v>
       </c>
@@ -28003,7 +28345,9 @@
       <c r="U381" t="n">
         <v>220.32</v>
       </c>
-      <c r="V381"/>
+      <c r="V381" t="n">
+        <v>2417.24736</v>
+      </c>
       <c r="W381" t="s">
         <v>529</v>
       </c>
@@ -28070,7 +28414,9 @@
       <c r="U382" t="n">
         <v>269.12</v>
       </c>
-      <c r="V382"/>
+      <c r="V382" t="n">
+        <v>3267.47562666667</v>
+      </c>
       <c r="W382" t="s">
         <v>529</v>
       </c>
@@ -28474,7 +28820,9 @@
       <c r="U388" t="n">
         <v>633.6</v>
       </c>
-      <c r="V388"/>
+      <c r="V388" t="n">
+        <v>58358.784</v>
+      </c>
       <c r="W388" t="s">
         <v>529</v>
       </c>
@@ -28539,7 +28887,9 @@
       <c r="U389" t="n">
         <v>807.36</v>
       </c>
-      <c r="V389"/>
+      <c r="V389" t="n">
+        <v>78419.41504</v>
+      </c>
       <c r="W389" t="s">
         <v>529</v>
       </c>
@@ -28606,7 +28956,9 @@
       <c r="U390" t="n">
         <v>585.12</v>
       </c>
-      <c r="V390"/>
+      <c r="V390" t="n">
+        <v>67611.78624</v>
+      </c>
       <c r="W390" t="s">
         <v>529</v>
       </c>
@@ -28736,7 +29088,9 @@
       <c r="U392" t="n">
         <v>917.28</v>
       </c>
-      <c r="V392"/>
+      <c r="V392" t="n">
+        <v>179728.17408</v>
+      </c>
       <c r="W392"/>
     </row>
     <row r="393">
@@ -28799,7 +29153,9 @@
       <c r="U393" t="n">
         <v>1737.12</v>
       </c>
-      <c r="V393"/>
+      <c r="V393" t="n">
+        <v>410182.67136</v>
+      </c>
       <c r="W393"/>
     </row>
     <row r="394">
@@ -28864,7 +29220,9 @@
       <c r="U394" t="n">
         <v>648.96</v>
       </c>
-      <c r="V394"/>
+      <c r="V394" t="n">
+        <v>9418.86122666667</v>
+      </c>
       <c r="W394"/>
     </row>
     <row r="395">
@@ -29031,7 +29389,7 @@
         <v>32</v>
       </c>
       <c r="K397" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L397"/>
       <c r="M397"/>
@@ -29096,7 +29454,7 @@
         <v>32</v>
       </c>
       <c r="K398" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L398" t="s">
         <v>40</v>
@@ -29126,7 +29484,9 @@
       <c r="U398" t="n">
         <v>983.68</v>
       </c>
-      <c r="V398"/>
+      <c r="V398" t="n">
+        <v>174617.627306667</v>
+      </c>
       <c r="W398"/>
     </row>
     <row r="399">
@@ -29161,7 +29521,7 @@
         <v>82</v>
       </c>
       <c r="K399" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L399"/>
       <c r="M399"/>
@@ -29358,7 +29718,7 @@
         <v>35</v>
       </c>
       <c r="K402" t="s">
-        <v>109</v>
+        <v>321</v>
       </c>
       <c r="L402"/>
       <c r="M402"/>
@@ -29386,7 +29746,9 @@
       <c r="U402" t="n">
         <v>924</v>
       </c>
-      <c r="V402"/>
+      <c r="V402" t="n">
+        <v>116054.4</v>
+      </c>
       <c r="W402"/>
     </row>
     <row r="403">
@@ -29451,7 +29813,9 @@
       <c r="U403" t="n">
         <v>427.68</v>
       </c>
-      <c r="V403"/>
+      <c r="V403" t="n">
+        <v>6455.94048</v>
+      </c>
       <c r="W403"/>
     </row>
     <row r="404">
@@ -29516,7 +29880,9 @@
       <c r="U404" t="n">
         <v>839.04</v>
       </c>
-      <c r="V404"/>
+      <c r="V404" t="n">
+        <v>129270.33344</v>
+      </c>
       <c r="W404"/>
     </row>
     <row r="405">
@@ -29551,7 +29917,7 @@
         <v>27</v>
       </c>
       <c r="K405" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L405" t="s">
         <v>40</v>
@@ -29750,7 +30116,7 @@
         <v>35</v>
       </c>
       <c r="K408" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L408" t="s">
         <v>140</v>
@@ -29821,7 +30187,7 @@
         <v>35</v>
       </c>
       <c r="K409" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L409" t="s">
         <v>140</v>
@@ -29892,7 +30258,7 @@
         <v>35</v>
       </c>
       <c r="K410" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L410"/>
       <c r="M410" t="s">
@@ -30265,7 +30631,9 @@
       <c r="U415" t="n">
         <v>772.48</v>
       </c>
-      <c r="V415"/>
+      <c r="V415" t="n">
+        <v>87967.9624533333</v>
+      </c>
       <c r="W415" t="s">
         <v>566</v>
       </c>
@@ -30892,7 +31260,9 @@
       <c r="U424" t="n">
         <v>94.24</v>
       </c>
-      <c r="V424"/>
+      <c r="V424" t="n">
+        <v>4892.43818666667</v>
+      </c>
       <c r="W424" t="s">
         <v>566</v>
       </c>
@@ -30961,7 +31331,9 @@
       <c r="U425" t="n">
         <v>74.24</v>
       </c>
-      <c r="V425"/>
+      <c r="V425" t="n">
+        <v>3605.49034666667</v>
+      </c>
       <c r="W425" t="s">
         <v>566</v>
       </c>
@@ -31030,7 +31402,9 @@
       <c r="U426" t="n">
         <v>92.48</v>
       </c>
-      <c r="V426"/>
+      <c r="V426" t="n">
+        <v>5265.68789333333</v>
+      </c>
       <c r="W426" t="s">
         <v>566</v>
       </c>
@@ -31302,7 +31676,9 @@
       <c r="U430" t="n">
         <v>89.76</v>
       </c>
-      <c r="V430"/>
+      <c r="V430" t="n">
+        <v>4960.49664</v>
+      </c>
       <c r="W430" t="s">
         <v>566</v>
       </c>
@@ -31369,7 +31745,9 @@
       <c r="U431" t="n">
         <v>108.8</v>
       </c>
-      <c r="V431"/>
+      <c r="V431" t="n">
+        <v>6194.92693333333</v>
+      </c>
       <c r="W431" t="s">
         <v>566</v>
       </c>
@@ -31940,7 +32318,7 @@
         <v>850</v>
       </c>
       <c r="I440" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J440" t="s">
         <v>35</v>
@@ -32074,7 +32452,7 @@
         <v>850</v>
       </c>
       <c r="I442" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J442" t="s">
         <v>27</v>
@@ -32342,7 +32720,7 @@
         <v>850</v>
       </c>
       <c r="I446" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J446" t="s">
         <v>27</v>
@@ -34803,7 +35181,7 @@
         <v>66</v>
       </c>
       <c r="K483" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L483" t="s">
         <v>40</v>
@@ -35339,7 +35717,7 @@
         <v>1050</v>
       </c>
       <c r="I491" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J491" t="s">
         <v>66</v>
@@ -35406,7 +35784,7 @@
         <v>1050</v>
       </c>
       <c r="I492" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J492" t="s">
         <v>27</v>
@@ -35473,7 +35851,7 @@
         <v>1050</v>
       </c>
       <c r="I493" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J493" t="s">
         <v>27</v>
@@ -35540,7 +35918,7 @@
         <v>1050</v>
       </c>
       <c r="I494" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J494" t="s">
         <v>66</v>
@@ -35808,7 +36186,7 @@
         <v>1050</v>
       </c>
       <c r="I498" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J498" t="s">
         <v>66</v>
@@ -35875,7 +36253,7 @@
         <v>1050</v>
       </c>
       <c r="I499" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J499" t="s">
         <v>27</v>
@@ -36007,7 +36385,7 @@
         <v>1050</v>
       </c>
       <c r="I501" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J501" t="s">
         <v>27</v>
@@ -36145,7 +36523,7 @@
         <v>66</v>
       </c>
       <c r="K503" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L503"/>
       <c r="M503"/>
@@ -36656,7 +37034,9 @@
       <c r="U510" t="n">
         <v>151.2</v>
       </c>
-      <c r="V510"/>
+      <c r="V510" t="n">
+        <v>1245.24864</v>
+      </c>
       <c r="W510" t="s">
         <v>656</v>
       </c>
@@ -39199,7 +39579,9 @@
       <c r="U547" t="n">
         <v>76.8</v>
       </c>
-      <c r="V547"/>
+      <c r="V547" t="n">
+        <v>3858.432</v>
+      </c>
       <c r="W547" t="s">
         <v>687</v>
       </c>
@@ -39674,7 +40056,9 @@
       <c r="U554" t="n">
         <v>915.2</v>
       </c>
-      <c r="V554"/>
+      <c r="V554" t="n">
+        <v>168592.042666667</v>
+      </c>
       <c r="W554"/>
     </row>
     <row r="555">
@@ -39739,7 +40123,9 @@
       <c r="U555" t="n">
         <v>426.24</v>
       </c>
-      <c r="V555"/>
+      <c r="V555" t="n">
+        <v>51394.31424</v>
+      </c>
       <c r="W555"/>
     </row>
     <row r="556">
@@ -39804,7 +40190,9 @@
       <c r="U556" t="n">
         <v>596.16</v>
       </c>
-      <c r="V556"/>
+      <c r="V556" t="n">
+        <v>80867.91168</v>
+      </c>
       <c r="W556"/>
     </row>
     <row r="557">
@@ -39839,7 +40227,7 @@
         <v>32</v>
       </c>
       <c r="K557" t="s">
-        <v>210</v>
+        <v>78</v>
       </c>
       <c r="L557" t="s">
         <v>140</v>
@@ -39871,7 +40259,9 @@
       <c r="U557" t="n">
         <v>382.72</v>
       </c>
-      <c r="V557"/>
+      <c r="V557" t="n">
+        <v>58965.4152533333</v>
+      </c>
       <c r="W557" t="s">
         <v>738</v>
       </c>
@@ -39938,7 +40328,9 @@
       <c r="U558" t="n">
         <v>1254.4</v>
       </c>
-      <c r="V558"/>
+      <c r="V558" t="n">
+        <v>168056.149333333</v>
+      </c>
       <c r="W558"/>
     </row>
     <row r="559">
@@ -40005,7 +40397,9 @@
       <c r="U559" t="n">
         <v>3617.6</v>
       </c>
-      <c r="V559"/>
+      <c r="V559" t="n">
+        <v>805750.459733333</v>
+      </c>
       <c r="W559" t="s">
         <v>741</v>
       </c>
@@ -40139,7 +40533,9 @@
       <c r="U561" t="n">
         <v>923.52</v>
       </c>
-      <c r="V561"/>
+      <c r="V561" t="n">
+        <v>57223.76192</v>
+      </c>
       <c r="W561" t="s">
         <v>744</v>
       </c>
@@ -40206,7 +40602,9 @@
       <c r="U562" t="n">
         <v>242.88</v>
       </c>
-      <c r="V562"/>
+      <c r="V562" t="n">
+        <v>2626.14528</v>
+      </c>
       <c r="W562"/>
     </row>
     <row r="563">
@@ -40436,7 +40834,7 @@
         <v>1150</v>
       </c>
       <c r="I566" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J566" t="s">
         <v>27</v>
@@ -40539,7 +40937,9 @@
       <c r="U567" t="n">
         <v>65.28</v>
       </c>
-      <c r="V567"/>
+      <c r="V567" t="n">
+        <v>367.823786666667</v>
+      </c>
       <c r="W567"/>
     </row>
     <row r="568">
@@ -41583,7 +41983,7 @@
       </c>
       <c r="J585"/>
       <c r="K585" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="L585"/>
       <c r="M585"/>
@@ -41721,7 +42121,9 @@
       <c r="U587" t="n">
         <v>0</v>
       </c>
-      <c r="V587"/>
+      <c r="V587" t="n">
+        <v>0</v>
+      </c>
       <c r="W587" t="s">
         <v>786</v>
       </c>
@@ -41776,7 +42178,9 @@
       <c r="U588" t="n">
         <v>0</v>
       </c>
-      <c r="V588"/>
+      <c r="V588" t="n">
+        <v>0</v>
+      </c>
       <c r="W588" t="s">
         <v>786</v>
       </c>
@@ -41831,7 +42235,9 @@
       <c r="U589" t="n">
         <v>0</v>
       </c>
-      <c r="V589"/>
+      <c r="V589" t="n">
+        <v>0</v>
+      </c>
       <c r="W589" t="s">
         <v>786</v>
       </c>
@@ -41886,7 +42292,9 @@
       <c r="U590" t="n">
         <v>0</v>
       </c>
-      <c r="V590"/>
+      <c r="V590" t="n">
+        <v>0</v>
+      </c>
       <c r="W590" t="s">
         <v>786</v>
       </c>
@@ -41941,7 +42349,9 @@
       <c r="U591" t="n">
         <v>0</v>
       </c>
-      <c r="V591"/>
+      <c r="V591" t="n">
+        <v>0</v>
+      </c>
       <c r="W591" t="s">
         <v>786</v>
       </c>
@@ -41996,7 +42406,9 @@
       <c r="U592" t="n">
         <v>0</v>
       </c>
-      <c r="V592"/>
+      <c r="V592" t="n">
+        <v>0</v>
+      </c>
       <c r="W592" t="s">
         <v>786</v>
       </c>
@@ -42051,7 +42463,9 @@
       <c r="U593" t="n">
         <v>0</v>
       </c>
-      <c r="V593"/>
+      <c r="V593" t="n">
+        <v>0</v>
+      </c>
       <c r="W593" t="s">
         <v>786</v>
       </c>
@@ -42686,7 +43100,9 @@
       <c r="U604" t="n">
         <v>376.96</v>
       </c>
-      <c r="V604"/>
+      <c r="V604" t="n">
+        <v>5343.05749333333</v>
+      </c>
       <c r="W604"/>
     </row>
     <row r="605">
@@ -42749,7 +43165,9 @@
       <c r="U605" t="n">
         <v>952.32</v>
       </c>
-      <c r="V605"/>
+      <c r="V605" t="n">
+        <v>21298.54464</v>
+      </c>
       <c r="W605"/>
     </row>
     <row r="606">
@@ -42812,7 +43230,9 @@
       <c r="U606" t="n">
         <v>936.96</v>
       </c>
-      <c r="V606"/>
+      <c r="V606" t="n">
+        <v>20835.5328</v>
+      </c>
       <c r="W606"/>
     </row>
     <row r="607">

</xml_diff>